<commit_message>
Brought 6x 1-bit I/O out into S1 connector, and added 25MHz clock with new buffer to same header. Layout and BOM updated.
</commit_message>
<xml_diff>
--- a/Manufacturing/V2/XMP16-V2-BOM.xlsx
+++ b/Manufacturing/V2/XMP16-V2-BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="12255" windowHeight="6045"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="XMP16_03" localSheetId="0">Sheet1!$A$9:$C$388</definedName>
+    <definedName name="XMP16_03" localSheetId="0">Sheet1!$A$9:$C$391</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="617">
   <si>
     <t>ref</t>
   </si>
@@ -1875,16 +1875,25 @@
   </si>
   <si>
     <t>R108</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>R110</t>
+  </si>
+  <si>
+    <t>U58</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2176,6 +2185,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2210,6 +2220,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2385,14 +2396,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F388"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="E190" sqref="E190"/>
+    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
+      <selection activeCell="B363" sqref="B363:F363"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
@@ -2400,7 +2411,7 @@
     <col min="5" max="5" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" s="50" t="s">
         <v>452</v>
       </c>
@@ -2409,31 +2420,31 @@
         <v>41127</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="51" t="s">
         <v>594</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="51"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>595</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2453,7 +2464,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25">
+    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2473,7 +2484,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.25">
+    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2493,7 +2504,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.25">
+    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2513,7 +2524,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.25">
+    <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2533,7 +2544,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.25">
+    <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2553,7 +2564,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.25">
+    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2573,7 +2584,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.25">
+    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -2593,7 +2604,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17.25" customHeight="1">
+    <row r="17" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -2613,7 +2624,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17.25">
+    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2633,7 +2644,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.25">
+    <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2653,7 +2664,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17.25">
+    <row r="20" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2673,7 +2684,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17.25">
+    <row r="21" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2693,7 +2704,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17.25">
+    <row r="22" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -2713,7 +2724,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17.25">
+    <row r="23" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -2733,7 +2744,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17.25">
+    <row r="24" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -2753,7 +2764,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17.25">
+    <row r="25" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2773,7 +2784,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17.25">
+    <row r="26" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2793,7 +2804,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17.25">
+    <row r="27" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -2813,7 +2824,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17.25">
+    <row r="28" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -2833,7 +2844,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17.25">
+    <row r="29" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2853,7 +2864,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17.25">
+    <row r="30" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -2873,7 +2884,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17.25">
+    <row r="31" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -2893,7 +2904,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="17.25">
+    <row r="32" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -2913,7 +2924,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="17.25">
+    <row r="33" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -2933,7 +2944,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17.25">
+    <row r="34" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -2953,7 +2964,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17.25">
+    <row r="35" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -2973,7 +2984,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="17.25">
+    <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -2993,7 +3004,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="17.25">
+    <row r="37" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -3013,7 +3024,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17.25">
+    <row r="38" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -3033,7 +3044,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17.25">
+    <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -3053,7 +3064,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="17.25">
+    <row r="40" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -3073,7 +3084,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17.25">
+    <row r="41" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -3093,7 +3104,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="17.25">
+    <row r="42" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -3113,7 +3124,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="17.25">
+    <row r="43" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -3133,7 +3144,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17.25">
+    <row r="44" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -3153,7 +3164,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17.25">
+    <row r="45" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -3173,7 +3184,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="17.25">
+    <row r="46" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -3193,7 +3204,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="17.25">
+    <row r="47" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -3213,7 +3224,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17.25">
+    <row r="48" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -3233,7 +3244,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="17.25">
+    <row r="49" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -3253,7 +3264,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="17.25">
+    <row r="50" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -3273,7 +3284,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="17.25">
+    <row r="51" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -3293,7 +3304,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="17.25">
+    <row r="52" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -3313,7 +3324,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="17.25">
+    <row r="53" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -3333,7 +3344,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="17.25">
+    <row r="54" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -3353,7 +3364,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="17.25">
+    <row r="55" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -3373,7 +3384,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="17.25">
+    <row r="56" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -3393,7 +3404,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="17.25">
+    <row r="57" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -3413,7 +3424,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="17.25">
+    <row r="58" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -3433,7 +3444,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="17.25">
+    <row r="59" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -3453,7 +3464,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="17.25">
+    <row r="60" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>53</v>
       </c>
@@ -3473,7 +3484,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="17.25">
+    <row r="61" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>54</v>
       </c>
@@ -3493,7 +3504,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="17.25">
+    <row r="62" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -3513,7 +3524,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="17.25">
+    <row r="63" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -3533,7 +3544,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="17.25">
+    <row r="64" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -3553,7 +3564,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="17.25">
+    <row r="65" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -3573,7 +3584,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="17.25">
+    <row r="66" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>59</v>
       </c>
@@ -3593,7 +3604,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="17.25">
+    <row r="67" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>60</v>
       </c>
@@ -3613,7 +3624,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="17.25">
+    <row r="68" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>61</v>
       </c>
@@ -3633,7 +3644,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="17.25">
+    <row r="69" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>62</v>
       </c>
@@ -3653,7 +3664,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="17.25">
+    <row r="70" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -3673,7 +3684,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="17.25">
+    <row r="71" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>64</v>
       </c>
@@ -3693,7 +3704,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="17.25">
+    <row r="72" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>65</v>
       </c>
@@ -3713,7 +3724,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="17.25">
+    <row r="73" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>66</v>
       </c>
@@ -3733,7 +3744,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="17.25">
+    <row r="74" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>67</v>
       </c>
@@ -3753,7 +3764,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="17.25">
+    <row r="75" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>68</v>
       </c>
@@ -3773,7 +3784,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="17.25">
+    <row r="76" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>69</v>
       </c>
@@ -3793,7 +3804,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="17.25">
+    <row r="77" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>70</v>
       </c>
@@ -3813,7 +3824,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="17.25">
+    <row r="78" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>71</v>
       </c>
@@ -3833,7 +3844,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="17.25">
+    <row r="79" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>72</v>
       </c>
@@ -3853,7 +3864,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="17.25">
+    <row r="80" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>73</v>
       </c>
@@ -3873,7 +3884,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="17.25">
+    <row r="81" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -3893,7 +3904,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="17.25">
+    <row r="82" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>75</v>
       </c>
@@ -3913,7 +3924,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="17.25">
+    <row r="83" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>76</v>
       </c>
@@ -3933,7 +3944,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="17.25">
+    <row r="84" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>77</v>
       </c>
@@ -3953,7 +3964,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="17.25">
+    <row r="85" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>78</v>
       </c>
@@ -3973,7 +3984,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="17.25">
+    <row r="86" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>79</v>
       </c>
@@ -3993,7 +4004,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="17.25">
+    <row r="87" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>80</v>
       </c>
@@ -4013,7 +4024,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="17.25">
+    <row r="88" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>81</v>
       </c>
@@ -4033,7 +4044,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="17.25">
+    <row r="89" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>82</v>
       </c>
@@ -4053,7 +4064,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="17.25">
+    <row r="90" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>83</v>
       </c>
@@ -4073,7 +4084,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="17.25">
+    <row r="91" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>84</v>
       </c>
@@ -4093,7 +4104,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="17.25">
+    <row r="92" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>85</v>
       </c>
@@ -4113,7 +4124,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="17.25">
+    <row r="93" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>86</v>
       </c>
@@ -4133,7 +4144,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="17.25">
+    <row r="94" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>87</v>
       </c>
@@ -4153,7 +4164,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="17.25">
+    <row r="95" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>88</v>
       </c>
@@ -4173,7 +4184,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="17.25">
+    <row r="96" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>89</v>
       </c>
@@ -4193,7 +4204,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="17.25">
+    <row r="97" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>90</v>
       </c>
@@ -4213,7 +4224,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="17.25">
+    <row r="98" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>91</v>
       </c>
@@ -4233,7 +4244,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="17.25">
+    <row r="99" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>92</v>
       </c>
@@ -4253,7 +4264,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="17.25">
+    <row r="100" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>93</v>
       </c>
@@ -4273,7 +4284,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="17.25">
+    <row r="101" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>94</v>
       </c>
@@ -4293,7 +4304,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="17.25">
+    <row r="102" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>95</v>
       </c>
@@ -4313,7 +4324,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="17.25">
+    <row r="103" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>96</v>
       </c>
@@ -4333,7 +4344,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="17.25">
+    <row r="104" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -4353,7 +4364,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="17.25">
+    <row r="105" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>98</v>
       </c>
@@ -4373,7 +4384,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="17.25">
+    <row r="106" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -4393,7 +4404,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="17.25">
+    <row r="107" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>100</v>
       </c>
@@ -4413,7 +4424,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="17.25">
+    <row r="108" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>101</v>
       </c>
@@ -4433,7 +4444,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="17.25">
+    <row r="109" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>102</v>
       </c>
@@ -4453,7 +4464,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="17.25">
+    <row r="110" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>103</v>
       </c>
@@ -4473,7 +4484,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="17.25">
+    <row r="111" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>104</v>
       </c>
@@ -4493,7 +4504,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="17.25">
+    <row r="112" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>105</v>
       </c>
@@ -4513,7 +4524,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="17.25">
+    <row r="113" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>106</v>
       </c>
@@ -4533,7 +4544,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="17.25">
+    <row r="114" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>107</v>
       </c>
@@ -4553,7 +4564,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="17.25">
+    <row r="115" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>108</v>
       </c>
@@ -4573,7 +4584,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="17.25">
+    <row r="116" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>109</v>
       </c>
@@ -4593,7 +4604,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="17.25">
+    <row r="117" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>110</v>
       </c>
@@ -4613,7 +4624,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="17.25">
+    <row r="118" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>111</v>
       </c>
@@ -4633,7 +4644,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="17.25">
+    <row r="119" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>112</v>
       </c>
@@ -4653,7 +4664,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="17.25">
+    <row r="120" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>115</v>
       </c>
@@ -4673,7 +4684,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="17.25">
+    <row r="121" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>116</v>
       </c>
@@ -4693,7 +4704,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="17.25">
+    <row r="122" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>117</v>
       </c>
@@ -4713,7 +4724,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="17.25">
+    <row r="123" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>118</v>
       </c>
@@ -4733,7 +4744,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="17.25">
+    <row r="124" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>119</v>
       </c>
@@ -4753,7 +4764,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="17.25">
+    <row r="125" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>120</v>
       </c>
@@ -4773,7 +4784,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="17.25">
+    <row r="126" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>121</v>
       </c>
@@ -4793,7 +4804,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="17.25">
+    <row r="127" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>122</v>
       </c>
@@ -4813,7 +4824,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="17.25">
+    <row r="128" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>123</v>
       </c>
@@ -4833,7 +4844,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="17.25">
+    <row r="129" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>124</v>
       </c>
@@ -4853,7 +4864,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="17.25">
+    <row r="130" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>125</v>
       </c>
@@ -4873,7 +4884,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="17.25">
+    <row r="131" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>126</v>
       </c>
@@ -4893,7 +4904,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="17.25">
+    <row r="132" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>127</v>
       </c>
@@ -4913,7 +4924,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="17.25">
+    <row r="133" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>128</v>
       </c>
@@ -4933,7 +4944,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="17.25">
+    <row r="134" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>129</v>
       </c>
@@ -4953,7 +4964,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="17.25">
+    <row r="135" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>130</v>
       </c>
@@ -4973,7 +4984,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="17.25">
+    <row r="136" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>131</v>
       </c>
@@ -4993,7 +5004,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="17.25">
+    <row r="137" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>132</v>
       </c>
@@ -5013,7 +5024,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="17.25">
+    <row r="138" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>133</v>
       </c>
@@ -5033,7 +5044,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="17.25">
+    <row r="139" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>134</v>
       </c>
@@ -5053,7 +5064,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="17.25">
+    <row r="140" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>135</v>
       </c>
@@ -5073,7 +5084,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="17.25">
+    <row r="141" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>136</v>
       </c>
@@ -5093,7 +5104,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="17.25">
+    <row r="142" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>137</v>
       </c>
@@ -5113,7 +5124,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="17.25">
+    <row r="143" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>138</v>
       </c>
@@ -5133,7 +5144,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="17.25">
+    <row r="144" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>139</v>
       </c>
@@ -5153,7 +5164,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="17.25">
+    <row r="145" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>140</v>
       </c>
@@ -5173,7 +5184,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="17.25">
+    <row r="146" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>141</v>
       </c>
@@ -5193,7 +5204,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="17.25">
+    <row r="147" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>142</v>
       </c>
@@ -5213,7 +5224,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="17.25">
+    <row r="148" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>143</v>
       </c>
@@ -5233,7 +5244,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="17.25">
+    <row r="149" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>144</v>
       </c>
@@ -5253,7 +5264,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="17.25">
+    <row r="150" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>145</v>
       </c>
@@ -5273,7 +5284,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="17.25">
+    <row r="151" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>146</v>
       </c>
@@ -5293,7 +5304,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="17.25">
+    <row r="152" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>147</v>
       </c>
@@ -5313,7 +5324,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="17.25">
+    <row r="153" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>148</v>
       </c>
@@ -5333,7 +5344,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="17.25">
+    <row r="154" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>597</v>
       </c>
@@ -5353,7 +5364,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="17.25">
+    <row r="155" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>598</v>
       </c>
@@ -5373,7 +5384,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="17.25">
+    <row r="156" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>599</v>
       </c>
@@ -5393,7 +5404,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="17.25">
+    <row r="157" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>600</v>
       </c>
@@ -5413,7 +5424,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="17.25">
+    <row r="158" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>601</v>
       </c>
@@ -5433,7 +5444,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="17.25">
+    <row r="159" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>602</v>
       </c>
@@ -5453,7 +5464,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="17.25">
+    <row r="160" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>603</v>
       </c>
@@ -5473,7 +5484,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="17.25">
+    <row r="161" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>604</v>
       </c>
@@ -5493,7 +5504,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="20" t="s">
         <v>149</v>
       </c>
@@ -5504,7 +5515,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="20" t="s">
         <v>152</v>
       </c>
@@ -5515,7 +5526,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="20" t="s">
         <v>153</v>
       </c>
@@ -5526,7 +5537,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="20" t="s">
         <v>154</v>
       </c>
@@ -5537,7 +5548,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="20" t="s">
         <v>155</v>
       </c>
@@ -5548,7 +5559,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="20" t="s">
         <v>156</v>
       </c>
@@ -5559,7 +5570,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="17.25">
+    <row r="168" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>157</v>
       </c>
@@ -5579,7 +5590,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="17.25">
+    <row r="169" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>160</v>
       </c>
@@ -5599,7 +5610,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="17.25">
+    <row r="170" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>162</v>
       </c>
@@ -5619,7 +5630,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="17.25">
+    <row r="171" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>163</v>
       </c>
@@ -5639,7 +5650,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="17.25">
+    <row r="172" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>164</v>
       </c>
@@ -5659,7 +5670,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="17.25">
+    <row r="173" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>165</v>
       </c>
@@ -5679,7 +5690,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="17.25">
+    <row r="174" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>166</v>
       </c>
@@ -5699,7 +5710,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="17.25">
+    <row r="175" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>169</v>
       </c>
@@ -5719,7 +5730,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="17.25">
+    <row r="176" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>171</v>
       </c>
@@ -5739,7 +5750,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="17.25">
+    <row r="177" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>172</v>
       </c>
@@ -5759,7 +5770,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="17.25">
+    <row r="178" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>173</v>
       </c>
@@ -5779,7 +5790,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="17.25">
+    <row r="179" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>176</v>
       </c>
@@ -5799,7 +5810,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="17.25">
+    <row r="180" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>177</v>
       </c>
@@ -5819,7 +5830,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="17.25">
+    <row r="181" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>178</v>
       </c>
@@ -5839,7 +5850,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="17.25">
+    <row r="182" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>179</v>
       </c>
@@ -5859,7 +5870,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="17.25">
+    <row r="183" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>180</v>
       </c>
@@ -5879,7 +5890,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="17.25">
+    <row r="184" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>181</v>
       </c>
@@ -5899,7 +5910,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="17.25">
+    <row r="185" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>182</v>
       </c>
@@ -5919,7 +5930,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>183</v>
       </c>
@@ -5930,7 +5941,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -5941,7 +5952,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>188</v>
       </c>
@@ -5952,7 +5963,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="17.25">
+    <row r="189" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>191</v>
       </c>
@@ -5972,7 +5983,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>193</v>
       </c>
@@ -5983,7 +5994,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>195</v>
       </c>
@@ -5994,7 +6005,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>198</v>
       </c>
@@ -6005,7 +6016,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>200</v>
       </c>
@@ -6016,7 +6027,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>202</v>
       </c>
@@ -6027,7 +6038,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>205</v>
       </c>
@@ -6038,7 +6049,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>206</v>
       </c>
@@ -6052,7 +6063,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>208</v>
       </c>
@@ -6066,7 +6077,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>210</v>
       </c>
@@ -6080,7 +6091,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>213</v>
       </c>
@@ -6094,7 +6105,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>214</v>
       </c>
@@ -6108,7 +6119,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>216</v>
       </c>
@@ -6122,7 +6133,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>218</v>
       </c>
@@ -6136,7 +6147,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>220</v>
       </c>
@@ -6150,7 +6161,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>222</v>
       </c>
@@ -6164,7 +6175,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>223</v>
       </c>
@@ -6178,7 +6189,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>224</v>
       </c>
@@ -6192,7 +6203,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>225</v>
       </c>
@@ -6206,7 +6217,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>226</v>
       </c>
@@ -6220,7 +6231,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>227</v>
       </c>
@@ -6234,7 +6245,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>228</v>
       </c>
@@ -6248,7 +6259,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>229</v>
       </c>
@@ -6262,7 +6273,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>230</v>
       </c>
@@ -6276,7 +6287,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="213" spans="1:5">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>231</v>
       </c>
@@ -6290,7 +6301,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="214" spans="1:5">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>233</v>
       </c>
@@ -6304,7 +6315,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="215" spans="1:5">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>234</v>
       </c>
@@ -6318,7 +6329,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>235</v>
       </c>
@@ -6332,7 +6343,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>236</v>
       </c>
@@ -6346,7 +6357,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="218" spans="1:5">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>237</v>
       </c>
@@ -6360,7 +6371,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="219" spans="1:5">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>238</v>
       </c>
@@ -6374,7 +6385,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>239</v>
       </c>
@@ -6388,7 +6399,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="221" spans="1:5">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>240</v>
       </c>
@@ -6402,7 +6413,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>241</v>
       </c>
@@ -6416,7 +6427,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="223" spans="1:5">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>243</v>
       </c>
@@ -6430,7 +6441,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="224" spans="1:5">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>244</v>
       </c>
@@ -6444,7 +6455,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="225" spans="1:5">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>245</v>
       </c>
@@ -6458,7 +6469,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>246</v>
       </c>
@@ -6472,7 +6483,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>247</v>
       </c>
@@ -6486,7 +6497,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>248</v>
       </c>
@@ -6500,7 +6511,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>249</v>
       </c>
@@ -6514,7 +6525,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>250</v>
       </c>
@@ -6528,7 +6539,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>251</v>
       </c>
@@ -6542,7 +6553,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>252</v>
       </c>
@@ -6556,7 +6567,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>253</v>
       </c>
@@ -6570,7 +6581,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>254</v>
       </c>
@@ -6584,7 +6595,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="235" spans="1:5">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>255</v>
       </c>
@@ -6598,7 +6609,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>256</v>
       </c>
@@ -6612,7 +6623,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>257</v>
       </c>
@@ -6626,7 +6637,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="238" spans="1:5">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>259</v>
       </c>
@@ -6640,7 +6651,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="239" spans="1:5">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>260</v>
       </c>
@@ -6654,7 +6665,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="240" spans="1:5">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>262</v>
       </c>
@@ -6668,7 +6679,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>263</v>
       </c>
@@ -6682,7 +6693,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="242" spans="1:5">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>264</v>
       </c>
@@ -6696,7 +6707,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="243" spans="1:5">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>265</v>
       </c>
@@ -6710,7 +6721,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="244" spans="1:5">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>267</v>
       </c>
@@ -6724,7 +6735,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="245" spans="1:5">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>268</v>
       </c>
@@ -6738,7 +6749,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="246" spans="1:5">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>269</v>
       </c>
@@ -6752,7 +6763,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="247" spans="1:5">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>270</v>
       </c>
@@ -6766,7 +6777,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="248" spans="1:5">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>271</v>
       </c>
@@ -6780,7 +6791,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="249" spans="1:5">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>272</v>
       </c>
@@ -6794,7 +6805,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="250" spans="1:5">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>273</v>
       </c>
@@ -6808,7 +6819,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="251" spans="1:5">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>274</v>
       </c>
@@ -6822,7 +6833,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="252" spans="1:5">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>275</v>
       </c>
@@ -6836,7 +6847,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="253" spans="1:5">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>276</v>
       </c>
@@ -6850,7 +6861,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="254" spans="1:5">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>277</v>
       </c>
@@ -6864,7 +6875,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="255" spans="1:5">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>278</v>
       </c>
@@ -6878,7 +6889,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="256" spans="1:5">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>279</v>
       </c>
@@ -6892,7 +6903,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="257" spans="1:5">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>280</v>
       </c>
@@ -6906,7 +6917,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="258" spans="1:5">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>281</v>
       </c>
@@ -6920,7 +6931,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="259" spans="1:5">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>282</v>
       </c>
@@ -6934,7 +6945,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="260" spans="1:5">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>283</v>
       </c>
@@ -6948,7 +6959,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="261" spans="1:5">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>284</v>
       </c>
@@ -6962,7 +6973,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="262" spans="1:5">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>285</v>
       </c>
@@ -6976,7 +6987,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="263" spans="1:5">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>286</v>
       </c>
@@ -6990,7 +7001,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="264" spans="1:5">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>287</v>
       </c>
@@ -7004,7 +7015,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="265" spans="1:5">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>288</v>
       </c>
@@ -7018,7 +7029,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="266" spans="1:5">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>289</v>
       </c>
@@ -7032,7 +7043,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="267" spans="1:5">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>290</v>
       </c>
@@ -7046,7 +7057,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="268" spans="1:5">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>291</v>
       </c>
@@ -7060,7 +7071,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="269" spans="1:5">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>292</v>
       </c>
@@ -7074,7 +7085,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="270" spans="1:5">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>293</v>
       </c>
@@ -7088,7 +7099,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="271" spans="1:5">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>294</v>
       </c>
@@ -7102,7 +7113,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="272" spans="1:5">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>295</v>
       </c>
@@ -7116,7 +7127,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="273" spans="1:5">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>296</v>
       </c>
@@ -7130,7 +7141,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="274" spans="1:5">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>297</v>
       </c>
@@ -7144,7 +7155,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="275" spans="1:5">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>298</v>
       </c>
@@ -7158,7 +7169,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="276" spans="1:5">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>299</v>
       </c>
@@ -7172,7 +7183,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="277" spans="1:5">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>300</v>
       </c>
@@ -7186,7 +7197,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="278" spans="1:5">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>301</v>
       </c>
@@ -7200,7 +7211,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="279" spans="1:5">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>302</v>
       </c>
@@ -7214,7 +7225,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="280" spans="1:5">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>303</v>
       </c>
@@ -7228,7 +7239,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="281" spans="1:5">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>304</v>
       </c>
@@ -7242,7 +7253,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="282" spans="1:5">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>305</v>
       </c>
@@ -7256,7 +7267,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="283" spans="1:5">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>306</v>
       </c>
@@ -7270,7 +7281,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="284" spans="1:5">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>307</v>
       </c>
@@ -7284,7 +7295,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="285" spans="1:5">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>308</v>
       </c>
@@ -7298,7 +7309,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="286" spans="1:5">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>309</v>
       </c>
@@ -7312,7 +7323,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="287" spans="1:5">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>310</v>
       </c>
@@ -7326,7 +7337,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="288" spans="1:5">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>311</v>
       </c>
@@ -7340,7 +7351,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="289" spans="1:6">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>313</v>
       </c>
@@ -7354,7 +7365,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="290" spans="1:6">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>314</v>
       </c>
@@ -7368,7 +7379,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="291" spans="1:6">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>317</v>
       </c>
@@ -7382,7 +7393,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="292" spans="1:6">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>318</v>
       </c>
@@ -7396,7 +7407,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="293" spans="1:6">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>319</v>
       </c>
@@ -7410,7 +7421,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="294" spans="1:6">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>320</v>
       </c>
@@ -7424,7 +7435,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="295" spans="1:6">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>321</v>
       </c>
@@ -7438,7 +7449,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="296" spans="1:6">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>606</v>
       </c>
@@ -7452,7 +7463,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="297" spans="1:6">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>607</v>
       </c>
@@ -7466,7 +7477,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="298" spans="1:6">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>608</v>
       </c>
@@ -7480,7 +7491,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="299" spans="1:6">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>609</v>
       </c>
@@ -7494,7 +7505,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="300" spans="1:6">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>610</v>
       </c>
@@ -7508,7 +7519,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="301" spans="1:6">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>611</v>
       </c>
@@ -7522,7 +7533,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="302" spans="1:6">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>612</v>
       </c>
@@ -7536,7 +7547,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="303" spans="1:6">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>613</v>
       </c>
@@ -7550,163 +7561,151 @@
         <v>541</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="17.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
+        <v>614</v>
+      </c>
+      <c r="B304" t="s">
+        <v>211</v>
+      </c>
+      <c r="C304" t="s">
+        <v>212</v>
+      </c>
+      <c r="E304" s="41" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>615</v>
+      </c>
+      <c r="B305" t="s">
+        <v>211</v>
+      </c>
+      <c r="C305" t="s">
+        <v>212</v>
+      </c>
+      <c r="E305" s="41" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
         <v>322</v>
       </c>
-      <c r="B304" t="s">
+      <c r="B306" t="s">
         <v>542</v>
       </c>
-      <c r="C304" t="s">
+      <c r="C306" t="s">
         <v>324</v>
       </c>
-      <c r="E304" s="25" t="s">
+      <c r="E306" s="25" t="s">
         <v>543</v>
       </c>
-      <c r="F304" s="26" t="s">
+      <c r="F306" s="26" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="17.25">
-      <c r="A305" t="s">
+    <row r="307" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
         <v>325</v>
       </c>
-      <c r="B305" t="s">
+      <c r="B307" t="s">
         <v>326</v>
       </c>
-      <c r="C305" t="s">
+      <c r="C307" t="s">
         <v>327</v>
       </c>
-      <c r="D305" t="s">
+      <c r="D307" t="s">
         <v>549</v>
       </c>
-      <c r="E305" s="3" t="s">
+      <c r="E307" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F305" s="43" t="s">
+      <c r="F307" s="43" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="306" spans="1:6" ht="17.25">
-      <c r="A306" t="s">
+    <row r="308" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
         <v>328</v>
       </c>
-      <c r="B306" t="s">
+      <c r="B308" t="s">
         <v>329</v>
       </c>
-      <c r="C306" t="s">
+      <c r="C308" t="s">
         <v>330</v>
       </c>
-      <c r="E306" s="29" t="s">
+      <c r="E308" s="29" t="s">
         <v>545</v>
       </c>
-      <c r="F306" s="31" t="s">
+      <c r="F308" s="31" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="307" spans="1:6" ht="15.75">
-      <c r="A307" t="s">
+    <row r="309" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
         <v>331</v>
       </c>
-      <c r="B307" t="s">
+      <c r="B309" t="s">
         <v>332</v>
       </c>
-      <c r="C307" t="s">
+      <c r="C309" t="s">
         <v>333</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D309" t="s">
         <v>552</v>
       </c>
-      <c r="E307" s="32" t="s">
+      <c r="E309" s="32" t="s">
         <v>550</v>
       </c>
-      <c r="F307" s="33" t="s">
+      <c r="F309" s="33" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="17.25">
-      <c r="A308" t="s">
+    <row r="310" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
         <v>334</v>
       </c>
-      <c r="B308" t="s">
+      <c r="B310" t="s">
         <v>335</v>
       </c>
-      <c r="C308" t="s">
+      <c r="C310" t="s">
         <v>336</v>
       </c>
-      <c r="D308" t="s">
+      <c r="D310" t="s">
         <v>555</v>
       </c>
-      <c r="E308" s="34" t="s">
+      <c r="E310" s="34" t="s">
         <v>553</v>
       </c>
-      <c r="F308" s="35" t="s">
+      <c r="F310" s="35" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="17.25">
-      <c r="A309" t="s">
+    <row r="311" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
         <v>337</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B311" t="s">
         <v>323</v>
       </c>
-      <c r="C309" t="s">
+      <c r="C311" t="s">
         <v>324</v>
       </c>
-      <c r="D309" t="s">
+      <c r="D311" t="s">
         <v>556</v>
       </c>
-      <c r="E309" s="27" t="s">
+      <c r="E311" s="27" t="s">
         <v>543</v>
       </c>
-      <c r="F309" s="28" t="s">
+      <c r="F311" s="28" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="17.25">
-      <c r="A310" t="s">
+    <row r="312" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
         <v>338</v>
-      </c>
-      <c r="B310" t="s">
-        <v>326</v>
-      </c>
-      <c r="C310" t="s">
-        <v>327</v>
-      </c>
-      <c r="D310" t="s">
-        <v>549</v>
-      </c>
-      <c r="E310" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F310" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" ht="17.25">
-      <c r="A311" t="s">
-        <v>339</v>
-      </c>
-      <c r="B311" t="s">
-        <v>326</v>
-      </c>
-      <c r="C311" t="s">
-        <v>327</v>
-      </c>
-      <c r="D311" t="s">
-        <v>549</v>
-      </c>
-      <c r="E311" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F311" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="312" spans="1:6" ht="17.25">
-      <c r="A312" t="s">
-        <v>340</v>
       </c>
       <c r="B312" t="s">
         <v>326</v>
@@ -7724,9 +7723,9 @@
         <v>547</v>
       </c>
     </row>
-    <row r="313" spans="1:6" ht="17.25">
+    <row r="313" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B313" t="s">
         <v>326</v>
@@ -7744,69 +7743,69 @@
         <v>547</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="17.25">
+    <row r="314" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B314" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="C314" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="D314" t="s">
-        <v>487</v>
-      </c>
-      <c r="E314" s="36" t="s">
-        <v>557</v>
-      </c>
-      <c r="F314" s="38" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" ht="17.25">
+        <v>549</v>
+      </c>
+      <c r="E314" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F314" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B315" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="C315" t="s">
         <v>327</v>
       </c>
       <c r="D315" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="E315" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="F315" s="37" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="316" spans="1:6" ht="17.25">
+        <v>548</v>
+      </c>
+      <c r="F315" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B316" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C316" t="s">
-        <v>327</v>
+        <v>344</v>
       </c>
       <c r="D316" t="s">
-        <v>555</v>
-      </c>
-      <c r="E316" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="F316" s="37" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="317" spans="1:6" ht="17.25">
+        <v>487</v>
+      </c>
+      <c r="E316" s="36" t="s">
+        <v>557</v>
+      </c>
+      <c r="F316" s="38" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B317" t="s">
         <v>346</v>
@@ -7824,9 +7823,9 @@
         <v>560</v>
       </c>
     </row>
-    <row r="318" spans="1:6" ht="17.25">
+    <row r="318" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B318" t="s">
         <v>346</v>
@@ -7844,109 +7843,109 @@
         <v>560</v>
       </c>
     </row>
-    <row r="319" spans="1:6" ht="17.25">
+    <row r="319" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B319" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="C319" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D319" t="s">
         <v>555</v>
       </c>
-      <c r="E319" s="36" t="s">
+      <c r="E319" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F319" s="37" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A320" t="s">
+        <v>349</v>
+      </c>
+      <c r="B320" t="s">
+        <v>346</v>
+      </c>
+      <c r="C320" t="s">
+        <v>327</v>
+      </c>
+      <c r="D320" t="s">
+        <v>555</v>
+      </c>
+      <c r="E320" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F320" s="37" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A321" t="s">
+        <v>350</v>
+      </c>
+      <c r="B321" t="s">
+        <v>335</v>
+      </c>
+      <c r="C321" t="s">
+        <v>336</v>
+      </c>
+      <c r="D321" t="s">
+        <v>555</v>
+      </c>
+      <c r="E321" s="36" t="s">
         <v>553</v>
       </c>
-      <c r="F319" s="38" t="s">
+      <c r="F321" s="38" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="320" spans="1:6" ht="17.25">
-      <c r="A320" t="s">
+    <row r="322" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A322" t="s">
         <v>351</v>
       </c>
-      <c r="B320" t="s">
+      <c r="B322" t="s">
         <v>352</v>
       </c>
-      <c r="C320" t="s">
+      <c r="C322" t="s">
         <v>353</v>
       </c>
-      <c r="D320" t="s">
+      <c r="D322" t="s">
         <v>563</v>
       </c>
-      <c r="E320" s="39" t="s">
+      <c r="E322" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F320" s="40" t="s">
+      <c r="F322" s="40" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="321" spans="1:6" ht="17.25">
-      <c r="A321" t="s">
+    <row r="323" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
         <v>354</v>
       </c>
-      <c r="B321" t="s">
+      <c r="B323" t="s">
         <v>355</v>
       </c>
-      <c r="C321" t="s">
+      <c r="C323" t="s">
         <v>356</v>
       </c>
-      <c r="D321" t="s">
+      <c r="D323" t="s">
         <v>565</v>
       </c>
-      <c r="E321" s="41" t="s">
+      <c r="E323" s="41" t="s">
         <v>355</v>
       </c>
-      <c r="F321" s="42" t="s">
+      <c r="F323" s="42" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="322" spans="1:6" ht="17.25">
-      <c r="A322" t="s">
+    <row r="324" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
         <v>357</v>
-      </c>
-      <c r="B322" t="s">
-        <v>326</v>
-      </c>
-      <c r="C322" t="s">
-        <v>327</v>
-      </c>
-      <c r="D322" t="s">
-        <v>549</v>
-      </c>
-      <c r="E322" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F322" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="323" spans="1:6" ht="17.25">
-      <c r="A323" t="s">
-        <v>358</v>
-      </c>
-      <c r="B323" t="s">
-        <v>359</v>
-      </c>
-      <c r="C323" t="s">
-        <v>327</v>
-      </c>
-      <c r="D323" t="s">
-        <v>549</v>
-      </c>
-      <c r="E323" s="44" t="s">
-        <v>566</v>
-      </c>
-      <c r="F323" s="45" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="324" spans="1:6" ht="17.25">
-      <c r="A324" t="s">
-        <v>360</v>
       </c>
       <c r="B324" t="s">
         <v>326</v>
@@ -7964,12 +7963,12 @@
         <v>547</v>
       </c>
     </row>
-    <row r="325" spans="1:6" ht="17.25">
+    <row r="325" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B325" t="s">
-        <v>326</v>
+        <v>359</v>
       </c>
       <c r="C325" t="s">
         <v>327</v>
@@ -7977,19 +7976,19 @@
       <c r="D325" t="s">
         <v>549</v>
       </c>
-      <c r="E325" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F325" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="326" spans="1:6" ht="17.25">
+      <c r="E325" s="44" t="s">
+        <v>566</v>
+      </c>
+      <c r="F325" s="45" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B326" t="s">
-        <v>359</v>
+        <v>326</v>
       </c>
       <c r="C326" t="s">
         <v>327</v>
@@ -7997,16 +7996,16 @@
       <c r="D326" t="s">
         <v>549</v>
       </c>
-      <c r="E326" s="44" t="s">
-        <v>566</v>
-      </c>
-      <c r="F326" s="45" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="327" spans="1:6" ht="17.25">
+      <c r="E326" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F326" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B327" t="s">
         <v>326</v>
@@ -8024,49 +8023,49 @@
         <v>547</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="15.75">
+    <row r="328" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
+        <v>362</v>
+      </c>
+      <c r="B328" t="s">
+        <v>359</v>
+      </c>
+      <c r="C328" t="s">
+        <v>327</v>
+      </c>
+      <c r="D328" t="s">
+        <v>549</v>
+      </c>
+      <c r="E328" s="44" t="s">
+        <v>566</v>
+      </c>
+      <c r="F328" s="45" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>363</v>
+      </c>
+      <c r="B329" t="s">
+        <v>326</v>
+      </c>
+      <c r="C329" t="s">
+        <v>327</v>
+      </c>
+      <c r="D329" t="s">
+        <v>549</v>
+      </c>
+      <c r="E329" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F329" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
         <v>364</v>
-      </c>
-      <c r="B328" t="s">
-        <v>571</v>
-      </c>
-      <c r="C328" t="s">
-        <v>365</v>
-      </c>
-      <c r="D328" t="s">
-        <v>568</v>
-      </c>
-      <c r="E328" s="47" t="s">
-        <v>569</v>
-      </c>
-      <c r="F328" s="46" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="329" spans="1:6" ht="15.75">
-      <c r="A329" t="s">
-        <v>366</v>
-      </c>
-      <c r="B329" t="s">
-        <v>571</v>
-      </c>
-      <c r="C329" t="s">
-        <v>365</v>
-      </c>
-      <c r="D329" t="s">
-        <v>568</v>
-      </c>
-      <c r="E329" s="47" t="s">
-        <v>569</v>
-      </c>
-      <c r="F329" s="46" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="330" spans="1:6" ht="15.75">
-      <c r="A330" t="s">
-        <v>367</v>
       </c>
       <c r="B330" t="s">
         <v>571</v>
@@ -8081,12 +8080,12 @@
         <v>569</v>
       </c>
       <c r="F330" s="46" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="331" spans="1:6" ht="15.75">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B331" t="s">
         <v>571</v>
@@ -8101,12 +8100,12 @@
         <v>569</v>
       </c>
       <c r="F331" s="46" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="332" spans="1:6" ht="15.75">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B332" t="s">
         <v>571</v>
@@ -8121,12 +8120,12 @@
         <v>569</v>
       </c>
       <c r="F332" s="46" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="333" spans="1:6" ht="15.75">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B333" t="s">
         <v>571</v>
@@ -8141,12 +8140,12 @@
         <v>569</v>
       </c>
       <c r="F333" s="46" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="334" spans="1:6" ht="15.75">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B334" t="s">
         <v>571</v>
@@ -8161,12 +8160,12 @@
         <v>569</v>
       </c>
       <c r="F334" s="46" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="335" spans="1:6" ht="15.75">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B335" t="s">
         <v>571</v>
@@ -8181,12 +8180,12 @@
         <v>569</v>
       </c>
       <c r="F335" s="46" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="336" spans="1:6" ht="15.75">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B336" t="s">
         <v>571</v>
@@ -8201,12 +8200,12 @@
         <v>569</v>
       </c>
       <c r="F336" s="46" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="337" spans="1:6" ht="15.75">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B337" t="s">
         <v>571</v>
@@ -8221,12 +8220,12 @@
         <v>569</v>
       </c>
       <c r="F337" s="46" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="338" spans="1:6" ht="15.75">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B338" t="s">
         <v>571</v>
@@ -8241,12 +8240,12 @@
         <v>569</v>
       </c>
       <c r="F338" s="46" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="339" spans="1:6" ht="15.75">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B339" t="s">
         <v>571</v>
@@ -8261,542 +8260,569 @@
         <v>569</v>
       </c>
       <c r="F339" s="46" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>375</v>
+      </c>
+      <c r="B340" t="s">
+        <v>571</v>
+      </c>
+      <c r="C340" t="s">
+        <v>365</v>
+      </c>
+      <c r="D340" t="s">
+        <v>568</v>
+      </c>
+      <c r="E340" s="47" t="s">
+        <v>569</v>
+      </c>
+      <c r="F340" s="46" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>376</v>
+      </c>
+      <c r="B341" t="s">
+        <v>571</v>
+      </c>
+      <c r="C341" t="s">
+        <v>365</v>
+      </c>
+      <c r="D341" t="s">
+        <v>568</v>
+      </c>
+      <c r="E341" s="47" t="s">
+        <v>569</v>
+      </c>
+      <c r="F341" s="46" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="340" spans="1:6" ht="17.25">
-      <c r="A340" t="s">
+    <row r="342" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
         <v>377</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B342" t="s">
         <v>326</v>
       </c>
-      <c r="C340" t="s">
+      <c r="C342" t="s">
         <v>327</v>
       </c>
-      <c r="D340" t="s">
+      <c r="D342" t="s">
         <v>549</v>
       </c>
-      <c r="E340" s="3" t="s">
+      <c r="E342" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F340" s="30" t="s">
+      <c r="F342" s="30" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="341" spans="1:6" ht="17.25">
-      <c r="A341" t="s">
+    <row r="343" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
         <v>378</v>
       </c>
-      <c r="B341" t="s">
+      <c r="B343" t="s">
         <v>326</v>
       </c>
-      <c r="C341" t="s">
+      <c r="C343" t="s">
         <v>327</v>
       </c>
-      <c r="D341" t="s">
+      <c r="D343" t="s">
         <v>549</v>
       </c>
-      <c r="E341" s="3" t="s">
+      <c r="E343" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F341" s="30" t="s">
+      <c r="F343" s="30" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="342" spans="1:6" ht="17.25">
-      <c r="A342" t="s">
+    <row r="344" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
         <v>379</v>
       </c>
-      <c r="B342" t="s">
+      <c r="B344" t="s">
         <v>352</v>
       </c>
-      <c r="C342" t="s">
+      <c r="C344" t="s">
         <v>353</v>
       </c>
-      <c r="D342" t="s">
+      <c r="D344" t="s">
         <v>563</v>
       </c>
-      <c r="E342" s="39" t="s">
+      <c r="E344" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F342" s="40" t="s">
+      <c r="F344" s="40" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="343" spans="1:6">
-      <c r="A343" s="23" t="s">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="B343" s="23" t="s">
+      <c r="B345" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C343" s="23" t="s">
+      <c r="C345" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D343" s="23" t="s">
+      <c r="D345" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E343" s="23" t="s">
+      <c r="E345" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F343" s="23" t="s">
+      <c r="F345" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="344" spans="1:6">
-      <c r="A344" s="23" t="s">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="B344" s="23" t="s">
+      <c r="B346" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C344" s="23" t="s">
+      <c r="C346" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D344" s="23" t="s">
+      <c r="D346" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E344" s="23" t="s">
+      <c r="E346" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F344" s="23" t="s">
+      <c r="F346" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="345" spans="1:6" ht="17.25">
-      <c r="A345" t="s">
+    <row r="347" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
         <v>384</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B347" t="s">
         <v>326</v>
       </c>
-      <c r="C345" t="s">
+      <c r="C347" t="s">
         <v>327</v>
       </c>
-      <c r="D345" t="s">
+      <c r="D347" t="s">
         <v>549</v>
       </c>
-      <c r="E345" s="3" t="s">
+      <c r="E347" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F345" s="30" t="s">
+      <c r="F347" s="30" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="346" spans="1:6" ht="17.25">
-      <c r="A346" t="s">
+    <row r="348" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
         <v>385</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B348" t="s">
         <v>326</v>
       </c>
-      <c r="C346" t="s">
+      <c r="C348" t="s">
         <v>327</v>
       </c>
-      <c r="D346" t="s">
+      <c r="D348" t="s">
         <v>549</v>
       </c>
-      <c r="E346" s="3" t="s">
+      <c r="E348" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F346" s="30" t="s">
+      <c r="F348" s="30" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="347" spans="1:6" ht="17.25">
-      <c r="A347" t="s">
+    <row r="349" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
         <v>386</v>
       </c>
-      <c r="B347" t="s">
+      <c r="B349" t="s">
         <v>352</v>
       </c>
-      <c r="C347" t="s">
+      <c r="C349" t="s">
         <v>353</v>
       </c>
-      <c r="D347" t="s">
+      <c r="D349" t="s">
         <v>563</v>
       </c>
-      <c r="E347" s="39" t="s">
+      <c r="E349" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F347" s="40" t="s">
+      <c r="F349" s="40" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="348" spans="1:6">
-      <c r="A348" s="23" t="s">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="B348" s="23" t="s">
+      <c r="B350" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C348" s="23" t="s">
+      <c r="C350" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D348" s="23" t="s">
+      <c r="D350" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E348" s="23" t="s">
+      <c r="E350" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F348" s="23" t="s">
+      <c r="F350" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="349" spans="1:6">
-      <c r="A349" s="23" t="s">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="B349" s="23" t="s">
+      <c r="B351" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C349" s="23" t="s">
+      <c r="C351" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D349" s="23" t="s">
+      <c r="D351" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E349" s="23" t="s">
+      <c r="E351" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F349" s="23" t="s">
+      <c r="F351" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="350" spans="1:6" ht="17.25">
-      <c r="A350" t="s">
+    <row r="352" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
         <v>389</v>
       </c>
-      <c r="B350" t="s">
+      <c r="B352" t="s">
         <v>326</v>
       </c>
-      <c r="C350" t="s">
+      <c r="C352" t="s">
         <v>327</v>
       </c>
-      <c r="D350" t="s">
+      <c r="D352" t="s">
         <v>549</v>
       </c>
-      <c r="E350" s="3" t="s">
+      <c r="E352" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F350" s="30" t="s">
+      <c r="F352" s="30" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="351" spans="1:6" ht="17.25">
-      <c r="A351" t="s">
+    <row r="353" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
         <v>390</v>
       </c>
-      <c r="B351" t="s">
+      <c r="B353" t="s">
         <v>326</v>
       </c>
-      <c r="C351" t="s">
+      <c r="C353" t="s">
         <v>327</v>
       </c>
-      <c r="D351" t="s">
+      <c r="D353" t="s">
         <v>549</v>
       </c>
-      <c r="E351" s="3" t="s">
+      <c r="E353" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F351" s="30" t="s">
+      <c r="F353" s="30" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="352" spans="1:6" ht="17.25">
-      <c r="A352" t="s">
+    <row r="354" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
         <v>391</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B354" t="s">
         <v>352</v>
       </c>
-      <c r="C352" t="s">
+      <c r="C354" t="s">
         <v>353</v>
       </c>
-      <c r="D352" t="s">
+      <c r="D354" t="s">
         <v>563</v>
       </c>
-      <c r="E352" s="39" t="s">
+      <c r="E354" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F352" s="40" t="s">
+      <c r="F354" s="40" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="353" spans="1:6">
-      <c r="A353" s="23" t="s">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="B353" s="23" t="s">
+      <c r="B355" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C353" s="23" t="s">
+      <c r="C355" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D353" s="23" t="s">
+      <c r="D355" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E353" s="23" t="s">
+      <c r="E355" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F353" s="23" t="s">
+      <c r="F355" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="354" spans="1:6">
-      <c r="A354" s="23" t="s">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="B354" s="23" t="s">
+      <c r="B356" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C354" s="23" t="s">
+      <c r="C356" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D354" s="23" t="s">
+      <c r="D356" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E354" s="23" t="s">
+      <c r="E356" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F354" s="23" t="s">
+      <c r="F356" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="355" spans="1:6" ht="17.25">
-      <c r="A355" t="s">
+    <row r="357" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
         <v>394</v>
       </c>
-      <c r="B355" t="s">
+      <c r="B357" t="s">
         <v>326</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C357" t="s">
         <v>327</v>
       </c>
-      <c r="D355" t="s">
+      <c r="D357" t="s">
         <v>549</v>
       </c>
-      <c r="E355" s="3" t="s">
+      <c r="E357" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F355" s="30" t="s">
+      <c r="F357" s="30" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="356" spans="1:6" ht="17.25">
-      <c r="A356" t="s">
+    <row r="358" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
         <v>395</v>
       </c>
-      <c r="B356" t="s">
+      <c r="B358" t="s">
         <v>326</v>
       </c>
-      <c r="C356" t="s">
+      <c r="C358" t="s">
         <v>327</v>
       </c>
-      <c r="D356" t="s">
+      <c r="D358" t="s">
         <v>549</v>
       </c>
-      <c r="E356" s="3" t="s">
+      <c r="E358" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F356" s="30" t="s">
+      <c r="F358" s="30" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="357" spans="1:6" ht="17.25">
-      <c r="A357" t="s">
+    <row r="359" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
         <v>396</v>
       </c>
-      <c r="B357" t="s">
+      <c r="B359" t="s">
         <v>352</v>
       </c>
-      <c r="C357" t="s">
+      <c r="C359" t="s">
         <v>353</v>
       </c>
-      <c r="D357" t="s">
+      <c r="D359" t="s">
         <v>563</v>
       </c>
-      <c r="E357" s="39" t="s">
+      <c r="E359" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F357" s="40" t="s">
+      <c r="F359" s="40" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="358" spans="1:6">
-      <c r="A358" s="23" t="s">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="B358" s="23" t="s">
+      <c r="B360" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C358" s="23" t="s">
+      <c r="C360" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D358" s="23" t="s">
+      <c r="D360" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E358" s="23" t="s">
+      <c r="E360" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F358" s="23" t="s">
+      <c r="F360" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="359" spans="1:6">
-      <c r="A359" s="23" t="s">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361" s="23" t="s">
         <v>398</v>
       </c>
-      <c r="B359" s="23" t="s">
+      <c r="B361" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C359" s="23" t="s">
+      <c r="C361" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D359" s="23" t="s">
+      <c r="D361" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E359" s="23" t="s">
+      <c r="E361" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F359" s="23" t="s">
+      <c r="F361" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="360" spans="1:6" ht="17.25">
-      <c r="A360" t="s">
+    <row r="362" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
         <v>399</v>
       </c>
-      <c r="B360" t="s">
+      <c r="B362" t="s">
         <v>400</v>
       </c>
-      <c r="C360" t="s">
+      <c r="C362" t="s">
         <v>588</v>
       </c>
-      <c r="D360" t="s">
+      <c r="D362" t="s">
         <v>586</v>
       </c>
-      <c r="E360" s="49" t="s">
+      <c r="E362" s="49" t="s">
         <v>587</v>
       </c>
-      <c r="F360" s="48" t="s">
+      <c r="F362" s="48" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="361" spans="1:6">
-      <c r="A361" t="s">
+    <row r="363" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>616</v>
+      </c>
+      <c r="B363" t="s">
+        <v>326</v>
+      </c>
+      <c r="C363" t="s">
+        <v>327</v>
+      </c>
+      <c r="D363" t="s">
+        <v>549</v>
+      </c>
+      <c r="E363" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F363" s="48" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
         <v>401</v>
       </c>
-      <c r="B361" s="20" t="s">
+      <c r="B364" s="20" t="s">
         <v>402</v>
-      </c>
-      <c r="C361" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="362" spans="1:6">
-      <c r="A362" t="s">
-        <v>404</v>
-      </c>
-      <c r="B362" s="20" t="s">
-        <v>405</v>
-      </c>
-      <c r="C362" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="363" spans="1:6">
-      <c r="A363" t="s">
-        <v>406</v>
-      </c>
-      <c r="B363" s="20" t="s">
-        <v>407</v>
-      </c>
-      <c r="C363" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="364" spans="1:6">
-      <c r="A364" t="s">
-        <v>408</v>
-      </c>
-      <c r="B364" s="20" t="s">
-        <v>409</v>
       </c>
       <c r="C364" s="20" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="365" spans="1:6">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="B365" s="20" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C365" s="20" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="366" spans="1:6">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B366" s="20" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="C366" s="20" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="367" spans="1:6">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B367" s="20" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C367" s="20" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="368" spans="1:6">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="B368" s="20" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C368" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="369" spans="1:3">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="B369" s="20" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="C369" s="20" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="370" spans="1:3">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="B370" s="20" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C370" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="371" spans="1:3">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B371" s="20" t="s">
         <v>418</v>
@@ -8805,108 +8831,108 @@
         <v>412</v>
       </c>
     </row>
-    <row r="372" spans="1:3">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B372" s="20" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C372" s="20" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="373" spans="1:3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B373" s="20" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C373" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="374" spans="1:3">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B374" s="20" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C374" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="375" spans="1:3">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B375" s="20" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C375" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="376" spans="1:3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B376" s="20" t="s">
-        <v>203</v>
+        <v>424</v>
       </c>
       <c r="C376" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="377" spans="1:3">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B377" s="20" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="C377" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="378" spans="1:3">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B378" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="C378" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>429</v>
+      </c>
+      <c r="B379" s="20" t="s">
         <v>203</v>
-      </c>
-      <c r="C378" s="20" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="379" spans="1:3">
-      <c r="A379" t="s">
-        <v>433</v>
-      </c>
-      <c r="B379" s="20" t="s">
-        <v>411</v>
       </c>
       <c r="C379" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="380" spans="1:3">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B380" s="20" t="s">
-        <v>203</v>
+        <v>431</v>
       </c>
       <c r="C380" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="381" spans="1:3">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B381" s="20" t="s">
         <v>203</v>
@@ -8915,80 +8941,113 @@
         <v>412</v>
       </c>
     </row>
-    <row r="382" spans="1:3">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B382" s="20" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="C382" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="383" spans="1:3">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
+        <v>434</v>
+      </c>
+      <c r="B383" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C383" s="20" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>435</v>
+      </c>
+      <c r="B384" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C384" s="20" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>436</v>
+      </c>
+      <c r="B385" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="C385" s="20" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
         <v>437</v>
       </c>
-      <c r="B383" s="20" t="s">
+      <c r="B386" s="20" t="s">
         <v>438</v>
-      </c>
-      <c r="C383" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="384" spans="1:3">
-      <c r="A384" t="s">
-        <v>439</v>
-      </c>
-      <c r="B384" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="C384" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="385" spans="1:3">
-      <c r="A385" t="s">
-        <v>441</v>
-      </c>
-      <c r="B385" s="20" t="s">
-        <v>442</v>
-      </c>
-      <c r="C385" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="386" spans="1:3">
-      <c r="A386" t="s">
-        <v>443</v>
-      </c>
-      <c r="B386" s="20" t="s">
-        <v>444</v>
       </c>
       <c r="C386" s="20" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="387" spans="1:3">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="B387" s="20" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="C387" s="20" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="388" spans="1:3">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
+        <v>441</v>
+      </c>
+      <c r="B388" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="C388" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>443</v>
+      </c>
+      <c r="B389" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="C389" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>445</v>
+      </c>
+      <c r="B390" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="C390" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
         <v>447</v>
       </c>
-      <c r="B388" s="20" t="s">
+      <c r="B391" s="20" t="s">
         <v>448</v>
       </c>
-      <c r="C388" s="20" t="s">
+      <c r="C391" s="20" t="s">
         <v>403</v>
       </c>
     </row>
@@ -9154,55 +9213,55 @@
     <hyperlink ref="F183" r:id="rId158"/>
     <hyperlink ref="F184" r:id="rId159"/>
     <hyperlink ref="F185" r:id="rId160"/>
-    <hyperlink ref="F304" r:id="rId161"/>
-    <hyperlink ref="F309" r:id="rId162"/>
-    <hyperlink ref="F306" r:id="rId163"/>
-    <hyperlink ref="F310" r:id="rId164"/>
-    <hyperlink ref="F311" r:id="rId165"/>
-    <hyperlink ref="F312" r:id="rId166"/>
-    <hyperlink ref="F313" r:id="rId167"/>
-    <hyperlink ref="F322" r:id="rId168"/>
-    <hyperlink ref="F324" r:id="rId169"/>
-    <hyperlink ref="F325" r:id="rId170"/>
-    <hyperlink ref="F327" r:id="rId171"/>
-    <hyperlink ref="F340" r:id="rId172"/>
-    <hyperlink ref="F341" r:id="rId173"/>
-    <hyperlink ref="F345" r:id="rId174"/>
-    <hyperlink ref="F346" r:id="rId175"/>
-    <hyperlink ref="F350" r:id="rId176"/>
-    <hyperlink ref="F351" r:id="rId177"/>
-    <hyperlink ref="F355" r:id="rId178"/>
-    <hyperlink ref="F356" r:id="rId179"/>
-    <hyperlink ref="F307" r:id="rId180"/>
-    <hyperlink ref="F308" r:id="rId181"/>
-    <hyperlink ref="F314" r:id="rId182"/>
-    <hyperlink ref="F315" r:id="rId183"/>
-    <hyperlink ref="F316" r:id="rId184"/>
-    <hyperlink ref="F317" r:id="rId185"/>
-    <hyperlink ref="F318" r:id="rId186"/>
-    <hyperlink ref="F319" r:id="rId187"/>
-    <hyperlink ref="F320" r:id="rId188"/>
-    <hyperlink ref="F342" r:id="rId189"/>
-    <hyperlink ref="F347" r:id="rId190"/>
-    <hyperlink ref="F352" r:id="rId191"/>
-    <hyperlink ref="F357" r:id="rId192"/>
-    <hyperlink ref="F321" r:id="rId193"/>
-    <hyperlink ref="F323" r:id="rId194"/>
-    <hyperlink ref="F326" r:id="rId195"/>
-    <hyperlink ref="F305" r:id="rId196"/>
-    <hyperlink ref="F328" r:id="rId197"/>
-    <hyperlink ref="F329" r:id="rId198" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F330" r:id="rId199" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F331" r:id="rId200" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F332" r:id="rId201" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F333" r:id="rId202" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F334" r:id="rId203" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F335" r:id="rId204" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F336" r:id="rId205" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F337" r:id="rId206" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F338" r:id="rId207" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F339" r:id="rId208" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F360" r:id="rId209"/>
+    <hyperlink ref="F306" r:id="rId161"/>
+    <hyperlink ref="F311" r:id="rId162"/>
+    <hyperlink ref="F308" r:id="rId163"/>
+    <hyperlink ref="F312" r:id="rId164"/>
+    <hyperlink ref="F313" r:id="rId165"/>
+    <hyperlink ref="F314" r:id="rId166"/>
+    <hyperlink ref="F315" r:id="rId167"/>
+    <hyperlink ref="F324" r:id="rId168"/>
+    <hyperlink ref="F326" r:id="rId169"/>
+    <hyperlink ref="F327" r:id="rId170"/>
+    <hyperlink ref="F329" r:id="rId171"/>
+    <hyperlink ref="F342" r:id="rId172"/>
+    <hyperlink ref="F343" r:id="rId173"/>
+    <hyperlink ref="F347" r:id="rId174"/>
+    <hyperlink ref="F348" r:id="rId175"/>
+    <hyperlink ref="F352" r:id="rId176"/>
+    <hyperlink ref="F353" r:id="rId177"/>
+    <hyperlink ref="F357" r:id="rId178"/>
+    <hyperlink ref="F358" r:id="rId179"/>
+    <hyperlink ref="F309" r:id="rId180"/>
+    <hyperlink ref="F310" r:id="rId181"/>
+    <hyperlink ref="F316" r:id="rId182"/>
+    <hyperlink ref="F317" r:id="rId183"/>
+    <hyperlink ref="F318" r:id="rId184"/>
+    <hyperlink ref="F319" r:id="rId185"/>
+    <hyperlink ref="F320" r:id="rId186"/>
+    <hyperlink ref="F321" r:id="rId187"/>
+    <hyperlink ref="F322" r:id="rId188"/>
+    <hyperlink ref="F344" r:id="rId189"/>
+    <hyperlink ref="F349" r:id="rId190"/>
+    <hyperlink ref="F354" r:id="rId191"/>
+    <hyperlink ref="F359" r:id="rId192"/>
+    <hyperlink ref="F323" r:id="rId193"/>
+    <hyperlink ref="F325" r:id="rId194"/>
+    <hyperlink ref="F328" r:id="rId195"/>
+    <hyperlink ref="F307" r:id="rId196"/>
+    <hyperlink ref="F330" r:id="rId197"/>
+    <hyperlink ref="F331" r:id="rId198" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F332" r:id="rId199" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F333" r:id="rId200" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F334" r:id="rId201" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F335" r:id="rId202" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F336" r:id="rId203" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F337" r:id="rId204" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F338" r:id="rId205" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F339" r:id="rId206" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F340" r:id="rId207" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F341" r:id="rId208" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F362" r:id="rId209"/>
     <hyperlink ref="F178" r:id="rId210"/>
     <hyperlink ref="F189" r:id="rId211"/>
     <hyperlink ref="F154" r:id="rId212" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
@@ -9213,31 +9272,32 @@
     <hyperlink ref="F159" r:id="rId217" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
     <hyperlink ref="F160" r:id="rId218" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
     <hyperlink ref="F161" r:id="rId219" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
+    <hyperlink ref="F363" r:id="rId220"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId220"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId221"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Unified header pattern for BL links with exception of 1-pin XLink offset. Now have 25MHz clock distribution + optional 3V3 power to header too.
</commit_message>
<xml_diff>
--- a/Manufacturing/V2/XMP16-V2-BOM.xlsx
+++ b/Manufacturing/V2/XMP16-V2-BOM.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="XMP16_03" localSheetId="0">Sheet1!$A$9:$C$391</definedName>
+    <definedName name="XMP16_03" localSheetId="0">Sheet1!$A$9:$C$395</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1963" uniqueCount="625">
   <si>
     <t>ref</t>
   </si>
@@ -1884,6 +1884,30 @@
   </si>
   <si>
     <t>U58</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>BL_3V3</t>
+  </si>
+  <si>
+    <t>BR_3V3</t>
+  </si>
+  <si>
+    <t>RST_BR</t>
+  </si>
+  <si>
+    <t>P26</t>
+  </si>
+  <si>
+    <t>B_CLK_EN</t>
   </si>
 </sst>
 </file>
@@ -2397,10 +2421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F391"/>
+  <dimension ref="A1:F395"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
-      <selection activeCell="B363" sqref="B363:F363"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="C199" sqref="C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6051,66 +6075,54 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>206</v>
-      </c>
-      <c r="B196" t="s">
-        <v>207</v>
-      </c>
-      <c r="C196" t="s">
-        <v>212</v>
-      </c>
-      <c r="E196" s="24" t="s">
-        <v>541</v>
+        <v>617</v>
+      </c>
+      <c r="B196" s="20" t="s">
+        <v>622</v>
+      </c>
+      <c r="C196" s="20" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>208</v>
-      </c>
-      <c r="B197" t="s">
-        <v>209</v>
-      </c>
-      <c r="C197" t="s">
-        <v>212</v>
-      </c>
-      <c r="E197" s="24" t="s">
-        <v>541</v>
+        <v>618</v>
+      </c>
+      <c r="B197" s="20" t="s">
+        <v>620</v>
+      </c>
+      <c r="C197" s="20" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>210</v>
-      </c>
-      <c r="B198" t="s">
-        <v>211</v>
-      </c>
-      <c r="C198" t="s">
-        <v>212</v>
-      </c>
-      <c r="E198" s="24" t="s">
-        <v>541</v>
+        <v>619</v>
+      </c>
+      <c r="B198" s="20" t="s">
+        <v>621</v>
+      </c>
+      <c r="C198" s="20" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>213</v>
-      </c>
-      <c r="B199" t="s">
-        <v>211</v>
-      </c>
-      <c r="C199" t="s">
-        <v>212</v>
-      </c>
-      <c r="E199" s="24" t="s">
-        <v>541</v>
+        <v>623</v>
+      </c>
+      <c r="B199" s="20" t="s">
+        <v>624</v>
+      </c>
+      <c r="C199" s="20" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B200" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C200" t="s">
         <v>212</v>
@@ -6121,10 +6133,10 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B201" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C201" t="s">
         <v>212</v>
@@ -6135,10 +6147,10 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B202" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C202" t="s">
         <v>212</v>
@@ -6149,10 +6161,10 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B203" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C203" t="s">
         <v>212</v>
@@ -6163,10 +6175,10 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B204" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C204" t="s">
         <v>212</v>
@@ -6177,10 +6189,10 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B205" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C205" t="s">
         <v>212</v>
@@ -6191,10 +6203,10 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B206" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="C206" t="s">
         <v>212</v>
@@ -6205,10 +6217,10 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B207" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C207" t="s">
         <v>212</v>
@@ -6219,7 +6231,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B208" t="s">
         <v>211</v>
@@ -6233,7 +6245,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B209" t="s">
         <v>211</v>
@@ -6247,7 +6259,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B210" t="s">
         <v>211</v>
@@ -6261,7 +6273,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B211" t="s">
         <v>211</v>
@@ -6275,10 +6287,10 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B212" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C212" t="s">
         <v>212</v>
@@ -6289,10 +6301,10 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B213" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="C213" t="s">
         <v>212</v>
@@ -6303,10 +6315,10 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B214" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C214" t="s">
         <v>212</v>
@@ -6317,10 +6329,10 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B215" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C215" t="s">
         <v>212</v>
@@ -6331,7 +6343,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B216" t="s">
         <v>221</v>
@@ -6345,10 +6357,10 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B217" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="C217" t="s">
         <v>212</v>
@@ -6359,10 +6371,10 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B218" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C218" t="s">
         <v>212</v>
@@ -6373,7 +6385,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B219" t="s">
         <v>221</v>
@@ -6387,10 +6399,10 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B220" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C220" t="s">
         <v>212</v>
@@ -6401,10 +6413,10 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B221" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C221" t="s">
         <v>212</v>
@@ -6415,10 +6427,10 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B222" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="C222" t="s">
         <v>212</v>
@@ -6429,10 +6441,10 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B223" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="C223" t="s">
         <v>212</v>
@@ -6443,7 +6455,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B224" t="s">
         <v>211</v>
@@ -6457,7 +6469,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B225" t="s">
         <v>211</v>
@@ -6471,10 +6483,10 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B226" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="C226" t="s">
         <v>212</v>
@@ -6485,10 +6497,10 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B227" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="C227" t="s">
         <v>212</v>
@@ -6499,7 +6511,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B228" t="s">
         <v>211</v>
@@ -6513,7 +6525,7 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B229" t="s">
         <v>211</v>
@@ -6527,7 +6539,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B230" t="s">
         <v>211</v>
@@ -6541,7 +6553,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B231" t="s">
         <v>211</v>
@@ -6555,7 +6567,7 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B232" t="s">
         <v>211</v>
@@ -6569,7 +6581,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B233" t="s">
         <v>211</v>
@@ -6583,7 +6595,7 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B234" t="s">
         <v>211</v>
@@ -6597,7 +6609,7 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B235" t="s">
         <v>211</v>
@@ -6611,7 +6623,7 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B236" t="s">
         <v>211</v>
@@ -6625,10 +6637,10 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B237" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="C237" t="s">
         <v>212</v>
@@ -6639,10 +6651,10 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B238" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C238" t="s">
         <v>212</v>
@@ -6653,10 +6665,10 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B239" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="C239" t="s">
         <v>212</v>
@@ -6667,10 +6679,10 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B240" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="C240" t="s">
         <v>212</v>
@@ -6681,10 +6693,10 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B241" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C241" t="s">
         <v>212</v>
@@ -6695,10 +6707,10 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B242" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="C242" t="s">
         <v>212</v>
@@ -6709,10 +6721,10 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B243" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C243" t="s">
         <v>212</v>
@@ -6723,7 +6735,7 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B244" t="s">
         <v>261</v>
@@ -6737,7 +6749,7 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B245" t="s">
         <v>261</v>
@@ -6751,7 +6763,7 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B246" t="s">
         <v>261</v>
@@ -6765,10 +6777,10 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B247" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C247" t="s">
         <v>212</v>
@@ -6779,10 +6791,10 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B248" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C248" t="s">
         <v>212</v>
@@ -6793,10 +6805,10 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B249" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C249" t="s">
         <v>212</v>
@@ -6807,10 +6819,10 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B250" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C250" t="s">
         <v>212</v>
@@ -6821,10 +6833,10 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B251" t="s">
-        <v>217</v>
+        <v>261</v>
       </c>
       <c r="C251" t="s">
         <v>212</v>
@@ -6835,10 +6847,10 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B252" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C252" t="s">
         <v>212</v>
@@ -6849,10 +6861,10 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B253" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="C253" t="s">
         <v>212</v>
@@ -6863,10 +6875,10 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B254" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C254" t="s">
         <v>212</v>
@@ -6877,10 +6889,10 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B255" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="C255" t="s">
         <v>212</v>
@@ -6891,10 +6903,10 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B256" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C256" t="s">
         <v>212</v>
@@ -6905,7 +6917,7 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B257" t="s">
         <v>261</v>
@@ -6919,7 +6931,7 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B258" t="s">
         <v>261</v>
@@ -6933,7 +6945,7 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B259" t="s">
         <v>261</v>
@@ -6947,10 +6959,10 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B260" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C260" t="s">
         <v>212</v>
@@ -6961,10 +6973,10 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B261" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C261" t="s">
         <v>212</v>
@@ -6975,10 +6987,10 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B262" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C262" t="s">
         <v>212</v>
@@ -6989,10 +7001,10 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B263" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C263" t="s">
         <v>212</v>
@@ -7003,10 +7015,10 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B264" t="s">
-        <v>217</v>
+        <v>261</v>
       </c>
       <c r="C264" t="s">
         <v>212</v>
@@ -7017,10 +7029,10 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B265" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C265" t="s">
         <v>212</v>
@@ -7031,10 +7043,10 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B266" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="C266" t="s">
         <v>212</v>
@@ -7045,10 +7057,10 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B267" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C267" t="s">
         <v>212</v>
@@ -7059,10 +7071,10 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B268" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="C268" t="s">
         <v>212</v>
@@ -7073,10 +7085,10 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B269" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C269" t="s">
         <v>212</v>
@@ -7087,7 +7099,7 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B270" t="s">
         <v>261</v>
@@ -7101,7 +7113,7 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B271" t="s">
         <v>261</v>
@@ -7115,7 +7127,7 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B272" t="s">
         <v>261</v>
@@ -7129,10 +7141,10 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B273" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C273" t="s">
         <v>212</v>
@@ -7143,10 +7155,10 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B274" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C274" t="s">
         <v>212</v>
@@ -7157,10 +7169,10 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B275" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C275" t="s">
         <v>212</v>
@@ -7171,10 +7183,10 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B276" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C276" t="s">
         <v>212</v>
@@ -7185,10 +7197,10 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B277" t="s">
-        <v>217</v>
+        <v>261</v>
       </c>
       <c r="C277" t="s">
         <v>212</v>
@@ -7199,10 +7211,10 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B278" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C278" t="s">
         <v>212</v>
@@ -7213,10 +7225,10 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B279" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="C279" t="s">
         <v>212</v>
@@ -7227,10 +7239,10 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B280" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C280" t="s">
         <v>212</v>
@@ -7241,10 +7253,10 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B281" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="C281" t="s">
         <v>212</v>
@@ -7255,10 +7267,10 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B282" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C282" t="s">
         <v>212</v>
@@ -7269,7 +7281,7 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B283" t="s">
         <v>261</v>
@@ -7283,7 +7295,7 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B284" t="s">
         <v>261</v>
@@ -7297,7 +7309,7 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B285" t="s">
         <v>261</v>
@@ -7311,10 +7323,10 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B286" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C286" t="s">
         <v>212</v>
@@ -7325,10 +7337,10 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B287" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C287" t="s">
         <v>212</v>
@@ -7339,10 +7351,10 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B288" t="s">
-        <v>312</v>
+        <v>261</v>
       </c>
       <c r="C288" t="s">
         <v>212</v>
@@ -7353,7 +7365,7 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B289" t="s">
         <v>261</v>
@@ -7367,13 +7379,13 @@
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B290" t="s">
-        <v>315</v>
+        <v>261</v>
       </c>
       <c r="C290" t="s">
-        <v>316</v>
+        <v>212</v>
       </c>
       <c r="E290" s="24" t="s">
         <v>541</v>
@@ -7381,13 +7393,13 @@
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B291" t="s">
-        <v>315</v>
+        <v>266</v>
       </c>
       <c r="C291" t="s">
-        <v>316</v>
+        <v>212</v>
       </c>
       <c r="E291" s="24" t="s">
         <v>541</v>
@@ -7395,13 +7407,13 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B292" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C292" t="s">
-        <v>316</v>
+        <v>212</v>
       </c>
       <c r="E292" s="24" t="s">
         <v>541</v>
@@ -7409,13 +7421,13 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B293" t="s">
-        <v>315</v>
+        <v>261</v>
       </c>
       <c r="C293" t="s">
-        <v>316</v>
+        <v>212</v>
       </c>
       <c r="E293" s="24" t="s">
         <v>541</v>
@@ -7423,7 +7435,7 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B294" t="s">
         <v>315</v>
@@ -7437,13 +7449,13 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B295" t="s">
-        <v>221</v>
+        <v>315</v>
       </c>
       <c r="C295" t="s">
-        <v>212</v>
+        <v>316</v>
       </c>
       <c r="E295" s="24" t="s">
         <v>541</v>
@@ -7451,63 +7463,63 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>606</v>
+        <v>318</v>
       </c>
       <c r="B296" t="s">
-        <v>261</v>
+        <v>315</v>
       </c>
       <c r="C296" t="s">
-        <v>212</v>
-      </c>
-      <c r="E296" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="E296" s="24" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>607</v>
+        <v>319</v>
       </c>
       <c r="B297" t="s">
-        <v>261</v>
+        <v>315</v>
       </c>
       <c r="C297" t="s">
-        <v>212</v>
-      </c>
-      <c r="E297" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="E297" s="24" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>608</v>
+        <v>320</v>
       </c>
       <c r="B298" t="s">
-        <v>261</v>
+        <v>315</v>
       </c>
       <c r="C298" t="s">
-        <v>212</v>
-      </c>
-      <c r="E298" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="E298" s="24" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>609</v>
+        <v>321</v>
       </c>
       <c r="B299" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="C299" t="s">
         <v>212</v>
       </c>
-      <c r="E299" s="41" t="s">
+      <c r="E299" s="24" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="B300" t="s">
         <v>261</v>
@@ -7521,7 +7533,7 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B301" t="s">
         <v>261</v>
@@ -7535,7 +7547,7 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B302" t="s">
         <v>261</v>
@@ -7549,7 +7561,7 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B303" t="s">
         <v>261</v>
@@ -7563,10 +7575,10 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="B304" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C304" t="s">
         <v>212</v>
@@ -7577,458 +7589,434 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
+        <v>611</v>
+      </c>
+      <c r="B305" t="s">
+        <v>261</v>
+      </c>
+      <c r="C305" t="s">
+        <v>212</v>
+      </c>
+      <c r="E305" s="41" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>612</v>
+      </c>
+      <c r="B306" t="s">
+        <v>261</v>
+      </c>
+      <c r="C306" t="s">
+        <v>212</v>
+      </c>
+      <c r="E306" s="41" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>613</v>
+      </c>
+      <c r="B307" t="s">
+        <v>261</v>
+      </c>
+      <c r="C307" t="s">
+        <v>212</v>
+      </c>
+      <c r="E307" s="41" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>614</v>
+      </c>
+      <c r="B308" t="s">
+        <v>211</v>
+      </c>
+      <c r="C308" t="s">
+        <v>212</v>
+      </c>
+      <c r="E308" s="41" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
         <v>615</v>
       </c>
-      <c r="B305" t="s">
+      <c r="B309" t="s">
         <v>211</v>
       </c>
-      <c r="C305" t="s">
-        <v>212</v>
-      </c>
-      <c r="E305" s="41" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="306" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A306" t="s">
-        <v>322</v>
-      </c>
-      <c r="B306" t="s">
-        <v>542</v>
-      </c>
-      <c r="C306" t="s">
-        <v>324</v>
-      </c>
-      <c r="E306" s="25" t="s">
-        <v>543</v>
-      </c>
-      <c r="F306" s="26" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="307" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A307" t="s">
-        <v>325</v>
-      </c>
-      <c r="B307" t="s">
-        <v>326</v>
-      </c>
-      <c r="C307" t="s">
-        <v>327</v>
-      </c>
-      <c r="D307" t="s">
-        <v>549</v>
-      </c>
-      <c r="E307" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F307" s="43" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="308" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A308" t="s">
-        <v>328</v>
-      </c>
-      <c r="B308" t="s">
-        <v>329</v>
-      </c>
-      <c r="C308" t="s">
-        <v>330</v>
-      </c>
-      <c r="E308" s="29" t="s">
-        <v>545</v>
-      </c>
-      <c r="F308" s="31" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
-        <v>331</v>
-      </c>
-      <c r="B309" t="s">
-        <v>332</v>
-      </c>
       <c r="C309" t="s">
-        <v>333</v>
-      </c>
-      <c r="D309" t="s">
-        <v>552</v>
-      </c>
-      <c r="E309" s="32" t="s">
-        <v>550</v>
-      </c>
-      <c r="F309" s="33" t="s">
-        <v>551</v>
+        <v>212</v>
+      </c>
+      <c r="E309" s="41" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="310" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="B310" t="s">
-        <v>335</v>
+        <v>542</v>
       </c>
       <c r="C310" t="s">
-        <v>336</v>
-      </c>
-      <c r="D310" t="s">
-        <v>555</v>
-      </c>
-      <c r="E310" s="34" t="s">
-        <v>553</v>
-      </c>
-      <c r="F310" s="35" t="s">
-        <v>554</v>
+        <v>324</v>
+      </c>
+      <c r="E310" s="25" t="s">
+        <v>543</v>
+      </c>
+      <c r="F310" s="26" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="311" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="B311" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C311" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D311" t="s">
-        <v>556</v>
-      </c>
-      <c r="E311" s="27" t="s">
-        <v>543</v>
-      </c>
-      <c r="F311" s="28" t="s">
-        <v>544</v>
+        <v>549</v>
+      </c>
+      <c r="E311" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F311" s="43" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="312" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="B312" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C312" t="s">
-        <v>327</v>
-      </c>
-      <c r="D312" t="s">
-        <v>549</v>
-      </c>
-      <c r="E312" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F312" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="313" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+      <c r="E312" s="29" t="s">
+        <v>545</v>
+      </c>
+      <c r="F312" s="31" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B313" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="C313" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="D313" t="s">
-        <v>549</v>
-      </c>
-      <c r="E313" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F313" s="30" t="s">
-        <v>547</v>
+        <v>552</v>
+      </c>
+      <c r="E313" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="F313" s="33" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="B314" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="C314" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="D314" t="s">
-        <v>549</v>
-      </c>
-      <c r="E314" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F314" s="30" t="s">
-        <v>547</v>
+        <v>555</v>
+      </c>
+      <c r="E314" s="34" t="s">
+        <v>553</v>
+      </c>
+      <c r="F314" s="35" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="315" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B315" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C315" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D315" t="s">
-        <v>549</v>
-      </c>
-      <c r="E315" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F315" s="30" t="s">
-        <v>547</v>
+        <v>556</v>
+      </c>
+      <c r="E315" s="27" t="s">
+        <v>543</v>
+      </c>
+      <c r="F315" s="28" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="316" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B316" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="C316" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="D316" t="s">
-        <v>487</v>
-      </c>
-      <c r="E316" s="36" t="s">
-        <v>557</v>
-      </c>
-      <c r="F316" s="38" t="s">
-        <v>558</v>
+        <v>549</v>
+      </c>
+      <c r="E316" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F316" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="317" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B317" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="C317" t="s">
         <v>327</v>
       </c>
       <c r="D317" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="E317" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="F317" s="37" t="s">
-        <v>560</v>
+        <v>548</v>
+      </c>
+      <c r="F317" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="318" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="B318" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="C318" t="s">
         <v>327</v>
       </c>
       <c r="D318" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="E318" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="F318" s="37" t="s">
-        <v>560</v>
+        <v>548</v>
+      </c>
+      <c r="F318" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="319" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="B319" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="C319" t="s">
         <v>327</v>
       </c>
       <c r="D319" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="E319" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="F319" s="37" t="s">
-        <v>560</v>
+        <v>548</v>
+      </c>
+      <c r="F319" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="320" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="B320" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C320" t="s">
-        <v>327</v>
+        <v>344</v>
       </c>
       <c r="D320" t="s">
-        <v>555</v>
-      </c>
-      <c r="E320" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="F320" s="37" t="s">
-        <v>560</v>
+        <v>487</v>
+      </c>
+      <c r="E320" s="36" t="s">
+        <v>557</v>
+      </c>
+      <c r="F320" s="38" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="321" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B321" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="C321" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D321" t="s">
         <v>555</v>
       </c>
-      <c r="E321" s="36" t="s">
-        <v>553</v>
-      </c>
-      <c r="F321" s="38" t="s">
-        <v>554</v>
+      <c r="E321" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F321" s="37" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="322" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B322" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C322" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="D322" t="s">
-        <v>563</v>
-      </c>
-      <c r="E322" s="39" t="s">
-        <v>561</v>
-      </c>
-      <c r="F322" s="40" t="s">
-        <v>562</v>
+        <v>555</v>
+      </c>
+      <c r="E322" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F322" s="37" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="323" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B323" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C323" t="s">
-        <v>356</v>
+        <v>327</v>
       </c>
       <c r="D323" t="s">
-        <v>565</v>
-      </c>
-      <c r="E323" s="41" t="s">
-        <v>355</v>
-      </c>
-      <c r="F323" s="42" t="s">
-        <v>564</v>
+        <v>555</v>
+      </c>
+      <c r="E323" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F323" s="37" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="324" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="B324" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="C324" t="s">
         <v>327</v>
       </c>
       <c r="D324" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="E324" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F324" s="30" t="s">
-        <v>547</v>
+        <v>559</v>
+      </c>
+      <c r="F324" s="37" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="325" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="B325" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="C325" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="D325" t="s">
-        <v>549</v>
-      </c>
-      <c r="E325" s="44" t="s">
-        <v>566</v>
-      </c>
-      <c r="F325" s="45" t="s">
-        <v>567</v>
+        <v>555</v>
+      </c>
+      <c r="E325" s="36" t="s">
+        <v>553</v>
+      </c>
+      <c r="F325" s="38" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="326" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="B326" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="C326" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="D326" t="s">
-        <v>549</v>
-      </c>
-      <c r="E326" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F326" s="30" t="s">
-        <v>547</v>
+        <v>563</v>
+      </c>
+      <c r="E326" s="39" t="s">
+        <v>561</v>
+      </c>
+      <c r="F326" s="40" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="327" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="B327" t="s">
-        <v>326</v>
+        <v>355</v>
       </c>
       <c r="C327" t="s">
-        <v>327</v>
+        <v>356</v>
       </c>
       <c r="D327" t="s">
-        <v>549</v>
-      </c>
-      <c r="E327" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F327" s="30" t="s">
-        <v>547</v>
+        <v>565</v>
+      </c>
+      <c r="E327" s="41" t="s">
+        <v>355</v>
+      </c>
+      <c r="F327" s="42" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="328" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B328" t="s">
-        <v>359</v>
+        <v>326</v>
       </c>
       <c r="C328" t="s">
         <v>327</v>
@@ -8036,19 +8024,19 @@
       <c r="D328" t="s">
         <v>549</v>
       </c>
-      <c r="E328" s="44" t="s">
-        <v>566</v>
-      </c>
-      <c r="F328" s="45" t="s">
-        <v>567</v>
+      <c r="E328" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F328" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="329" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B329" t="s">
-        <v>326</v>
+        <v>359</v>
       </c>
       <c r="C329" t="s">
         <v>327</v>
@@ -8056,96 +8044,96 @@
       <c r="D329" t="s">
         <v>549</v>
       </c>
-      <c r="E329" s="3" t="s">
+      <c r="E329" s="44" t="s">
+        <v>566</v>
+      </c>
+      <c r="F329" s="45" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>360</v>
+      </c>
+      <c r="B330" t="s">
+        <v>326</v>
+      </c>
+      <c r="C330" t="s">
+        <v>327</v>
+      </c>
+      <c r="D330" t="s">
+        <v>549</v>
+      </c>
+      <c r="E330" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F329" s="30" t="s">
+      <c r="F330" s="30" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A330" t="s">
-        <v>364</v>
-      </c>
-      <c r="B330" t="s">
-        <v>571</v>
-      </c>
-      <c r="C330" t="s">
-        <v>365</v>
-      </c>
-      <c r="D330" t="s">
-        <v>568</v>
-      </c>
-      <c r="E330" s="47" t="s">
-        <v>569</v>
-      </c>
-      <c r="F330" s="46" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="331" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B331" t="s">
-        <v>571</v>
+        <v>326</v>
       </c>
       <c r="C331" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
       <c r="D331" t="s">
-        <v>568</v>
-      </c>
-      <c r="E331" s="47" t="s">
-        <v>569</v>
-      </c>
-      <c r="F331" s="46" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="332" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+      <c r="E331" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F331" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B332" t="s">
-        <v>571</v>
+        <v>359</v>
       </c>
       <c r="C332" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
       <c r="D332" t="s">
-        <v>568</v>
-      </c>
-      <c r="E332" s="47" t="s">
-        <v>569</v>
-      </c>
-      <c r="F332" s="46" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="333" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+      <c r="E332" s="44" t="s">
+        <v>566</v>
+      </c>
+      <c r="F332" s="45" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B333" t="s">
-        <v>571</v>
+        <v>326</v>
       </c>
       <c r="C333" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
       <c r="D333" t="s">
-        <v>568</v>
-      </c>
-      <c r="E333" s="47" t="s">
-        <v>569</v>
-      </c>
-      <c r="F333" s="46" t="s">
-        <v>574</v>
+        <v>549</v>
+      </c>
+      <c r="E333" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F333" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="334" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B334" t="s">
         <v>571</v>
@@ -8160,12 +8148,12 @@
         <v>569</v>
       </c>
       <c r="F334" s="46" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="335" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B335" t="s">
         <v>571</v>
@@ -8180,12 +8168,12 @@
         <v>569</v>
       </c>
       <c r="F335" s="46" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="336" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B336" t="s">
         <v>571</v>
@@ -8200,12 +8188,12 @@
         <v>569</v>
       </c>
       <c r="F336" s="46" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="337" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B337" t="s">
         <v>571</v>
@@ -8220,12 +8208,12 @@
         <v>569</v>
       </c>
       <c r="F337" s="46" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="338" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B338" t="s">
         <v>571</v>
@@ -8240,12 +8228,12 @@
         <v>569</v>
       </c>
       <c r="F338" s="46" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="339" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B339" t="s">
         <v>571</v>
@@ -8260,12 +8248,12 @@
         <v>569</v>
       </c>
       <c r="F339" s="46" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="340" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B340" t="s">
         <v>571</v>
@@ -8280,12 +8268,12 @@
         <v>569</v>
       </c>
       <c r="F340" s="46" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="341" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B341" t="s">
         <v>571</v>
@@ -8300,112 +8288,112 @@
         <v>569</v>
       </c>
       <c r="F341" s="46" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>373</v>
+      </c>
+      <c r="B342" t="s">
+        <v>571</v>
+      </c>
+      <c r="C342" t="s">
+        <v>365</v>
+      </c>
+      <c r="D342" t="s">
+        <v>568</v>
+      </c>
+      <c r="E342" s="47" t="s">
+        <v>569</v>
+      </c>
+      <c r="F342" s="46" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>374</v>
+      </c>
+      <c r="B343" t="s">
+        <v>571</v>
+      </c>
+      <c r="C343" t="s">
+        <v>365</v>
+      </c>
+      <c r="D343" t="s">
+        <v>568</v>
+      </c>
+      <c r="E343" s="47" t="s">
+        <v>569</v>
+      </c>
+      <c r="F343" s="46" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>375</v>
+      </c>
+      <c r="B344" t="s">
+        <v>571</v>
+      </c>
+      <c r="C344" t="s">
+        <v>365</v>
+      </c>
+      <c r="D344" t="s">
+        <v>568</v>
+      </c>
+      <c r="E344" s="47" t="s">
+        <v>569</v>
+      </c>
+      <c r="F344" s="46" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>376</v>
+      </c>
+      <c r="B345" t="s">
+        <v>571</v>
+      </c>
+      <c r="C345" t="s">
+        <v>365</v>
+      </c>
+      <c r="D345" t="s">
+        <v>568</v>
+      </c>
+      <c r="E345" s="47" t="s">
+        <v>569</v>
+      </c>
+      <c r="F345" s="46" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="342" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A342" t="s">
+    <row r="346" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
         <v>377</v>
       </c>
-      <c r="B342" t="s">
+      <c r="B346" t="s">
         <v>326</v>
       </c>
-      <c r="C342" t="s">
+      <c r="C346" t="s">
         <v>327</v>
       </c>
-      <c r="D342" t="s">
+      <c r="D346" t="s">
         <v>549</v>
       </c>
-      <c r="E342" s="3" t="s">
+      <c r="E346" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F342" s="30" t="s">
+      <c r="F346" s="30" t="s">
         <v>547</v>
-      </c>
-    </row>
-    <row r="343" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A343" t="s">
-        <v>378</v>
-      </c>
-      <c r="B343" t="s">
-        <v>326</v>
-      </c>
-      <c r="C343" t="s">
-        <v>327</v>
-      </c>
-      <c r="D343" t="s">
-        <v>549</v>
-      </c>
-      <c r="E343" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F343" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="344" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A344" t="s">
-        <v>379</v>
-      </c>
-      <c r="B344" t="s">
-        <v>352</v>
-      </c>
-      <c r="C344" t="s">
-        <v>353</v>
-      </c>
-      <c r="D344" t="s">
-        <v>563</v>
-      </c>
-      <c r="E344" s="39" t="s">
-        <v>561</v>
-      </c>
-      <c r="F344" s="40" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A345" s="23" t="s">
-        <v>380</v>
-      </c>
-      <c r="B345" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="C345" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="D345" s="23" t="s">
-        <v>583</v>
-      </c>
-      <c r="E345" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="F345" s="23" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A346" s="23" t="s">
-        <v>383</v>
-      </c>
-      <c r="B346" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="C346" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="D346" s="23" t="s">
-        <v>583</v>
-      </c>
-      <c r="E346" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="F346" s="23" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="347" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="B347" t="s">
         <v>326</v>
@@ -8425,47 +8413,47 @@
     </row>
     <row r="348" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B348" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="C348" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="D348" t="s">
-        <v>549</v>
-      </c>
-      <c r="E348" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F348" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="349" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A349" t="s">
-        <v>386</v>
-      </c>
-      <c r="B349" t="s">
-        <v>352</v>
-      </c>
-      <c r="C349" t="s">
-        <v>353</v>
-      </c>
-      <c r="D349" t="s">
         <v>563</v>
       </c>
-      <c r="E349" s="39" t="s">
+      <c r="E348" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F349" s="40" t="s">
+      <c r="F348" s="40" t="s">
         <v>562</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="B349" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="C349" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="D349" s="23" t="s">
+        <v>583</v>
+      </c>
+      <c r="E349" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="F349" s="23" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" s="23" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B350" s="23" t="s">
         <v>381</v>
@@ -8483,29 +8471,29 @@
         <v>584</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A351" s="23" t="s">
-        <v>388</v>
-      </c>
-      <c r="B351" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="C351" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="D351" s="23" t="s">
-        <v>583</v>
-      </c>
-      <c r="E351" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="F351" s="23" t="s">
-        <v>584</v>
+    <row r="351" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>384</v>
+      </c>
+      <c r="B351" t="s">
+        <v>326</v>
+      </c>
+      <c r="C351" t="s">
+        <v>327</v>
+      </c>
+      <c r="D351" t="s">
+        <v>549</v>
+      </c>
+      <c r="E351" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F351" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="352" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B352" t="s">
         <v>326</v>
@@ -8525,47 +8513,47 @@
     </row>
     <row r="353" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B353" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="C353" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="D353" t="s">
-        <v>549</v>
-      </c>
-      <c r="E353" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F353" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="354" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A354" t="s">
-        <v>391</v>
-      </c>
-      <c r="B354" t="s">
-        <v>352</v>
-      </c>
-      <c r="C354" t="s">
-        <v>353</v>
-      </c>
-      <c r="D354" t="s">
         <v>563</v>
       </c>
-      <c r="E354" s="39" t="s">
+      <c r="E353" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F354" s="40" t="s">
+      <c r="F353" s="40" t="s">
         <v>562</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="B354" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="C354" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="D354" s="23" t="s">
+        <v>583</v>
+      </c>
+      <c r="E354" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="F354" s="23" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355" s="23" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B355" s="23" t="s">
         <v>381</v>
@@ -8583,29 +8571,29 @@
         <v>584</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A356" s="23" t="s">
-        <v>393</v>
-      </c>
-      <c r="B356" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="C356" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="D356" s="23" t="s">
-        <v>583</v>
-      </c>
-      <c r="E356" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="F356" s="23" t="s">
-        <v>584</v>
+    <row r="356" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>389</v>
+      </c>
+      <c r="B356" t="s">
+        <v>326</v>
+      </c>
+      <c r="C356" t="s">
+        <v>327</v>
+      </c>
+      <c r="D356" t="s">
+        <v>549</v>
+      </c>
+      <c r="E356" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F356" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="357" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B357" t="s">
         <v>326</v>
@@ -8625,47 +8613,47 @@
     </row>
     <row r="358" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B358" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="C358" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="D358" t="s">
-        <v>549</v>
-      </c>
-      <c r="E358" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F358" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="359" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A359" t="s">
-        <v>396</v>
-      </c>
-      <c r="B359" t="s">
-        <v>352</v>
-      </c>
-      <c r="C359" t="s">
-        <v>353</v>
-      </c>
-      <c r="D359" t="s">
         <v>563</v>
       </c>
-      <c r="E359" s="39" t="s">
+      <c r="E358" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F359" s="40" t="s">
+      <c r="F358" s="40" t="s">
         <v>562</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359" s="23" t="s">
+        <v>392</v>
+      </c>
+      <c r="B359" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="C359" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="D359" s="23" t="s">
+        <v>583</v>
+      </c>
+      <c r="E359" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="F359" s="23" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" s="23" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B360" s="23" t="s">
         <v>381</v>
@@ -8683,127 +8671,163 @@
         <v>584</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A361" s="23" t="s">
-        <v>398</v>
-      </c>
-      <c r="B361" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="C361" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="D361" s="23" t="s">
-        <v>583</v>
-      </c>
-      <c r="E361" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="F361" s="23" t="s">
-        <v>584</v>
+    <row r="361" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>394</v>
+      </c>
+      <c r="B361" t="s">
+        <v>326</v>
+      </c>
+      <c r="C361" t="s">
+        <v>327</v>
+      </c>
+      <c r="D361" t="s">
+        <v>549</v>
+      </c>
+      <c r="E361" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F361" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="362" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B362" t="s">
-        <v>400</v>
+        <v>326</v>
       </c>
       <c r="C362" t="s">
-        <v>588</v>
+        <v>327</v>
       </c>
       <c r="D362" t="s">
-        <v>586</v>
-      </c>
-      <c r="E362" s="49" t="s">
-        <v>587</v>
-      </c>
-      <c r="F362" s="48" t="s">
-        <v>585</v>
+        <v>549</v>
+      </c>
+      <c r="E362" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F362" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="363" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
+        <v>396</v>
+      </c>
+      <c r="B363" t="s">
+        <v>352</v>
+      </c>
+      <c r="C363" t="s">
+        <v>353</v>
+      </c>
+      <c r="D363" t="s">
+        <v>563</v>
+      </c>
+      <c r="E363" s="39" t="s">
+        <v>561</v>
+      </c>
+      <c r="F363" s="40" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364" s="23" t="s">
+        <v>397</v>
+      </c>
+      <c r="B364" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="C364" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="D364" s="23" t="s">
+        <v>583</v>
+      </c>
+      <c r="E364" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="F364" s="23" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="B365" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="C365" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="D365" s="23" t="s">
+        <v>583</v>
+      </c>
+      <c r="E365" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="F365" s="23" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>399</v>
+      </c>
+      <c r="B366" t="s">
+        <v>400</v>
+      </c>
+      <c r="C366" t="s">
+        <v>588</v>
+      </c>
+      <c r="D366" t="s">
+        <v>586</v>
+      </c>
+      <c r="E366" s="49" t="s">
+        <v>587</v>
+      </c>
+      <c r="F366" s="48" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
         <v>616</v>
       </c>
-      <c r="B363" t="s">
+      <c r="B367" t="s">
         <v>326</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C367" t="s">
         <v>327</v>
       </c>
-      <c r="D363" t="s">
+      <c r="D367" t="s">
         <v>549</v>
       </c>
-      <c r="E363" s="3" t="s">
+      <c r="E367" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F363" s="48" t="s">
+      <c r="F367" s="48" t="s">
         <v>547</v>
-      </c>
-    </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
-        <v>401</v>
-      </c>
-      <c r="B364" s="20" t="s">
-        <v>402</v>
-      </c>
-      <c r="C364" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A365" t="s">
-        <v>404</v>
-      </c>
-      <c r="B365" s="20" t="s">
-        <v>405</v>
-      </c>
-      <c r="C365" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
-        <v>406</v>
-      </c>
-      <c r="B366" s="20" t="s">
-        <v>407</v>
-      </c>
-      <c r="C366" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
-        <v>408</v>
-      </c>
-      <c r="B367" s="20" t="s">
-        <v>409</v>
-      </c>
-      <c r="C367" s="20" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="B368" s="20" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="C368" s="20" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B369" s="20" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C369" s="20" t="s">
         <v>403</v>
@@ -8811,54 +8835,54 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="B370" s="20" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="C370" s="20" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="B371" s="20" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C371" s="20" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="B372" s="20" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C372" s="20" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B373" s="20" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C373" s="20" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B374" s="20" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C374" s="20" t="s">
         <v>412</v>
@@ -8866,10 +8890,10 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="B375" s="20" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C375" s="20" t="s">
         <v>412</v>
@@ -8877,21 +8901,21 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="B376" s="20" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C376" s="20" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B377" s="20" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C377" s="20" t="s">
         <v>412</v>
@@ -8899,21 +8923,21 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B378" s="20" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="C378" s="20" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="B379" s="20" t="s">
-        <v>203</v>
+        <v>424</v>
       </c>
       <c r="C379" s="20" t="s">
         <v>412</v>
@@ -8921,10 +8945,10 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B380" s="20" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="C380" s="20" t="s">
         <v>412</v>
@@ -8932,10 +8956,10 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="B381" s="20" t="s">
-        <v>203</v>
+        <v>420</v>
       </c>
       <c r="C381" s="20" t="s">
         <v>412</v>
@@ -8943,18 +8967,18 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B382" s="20" t="s">
-        <v>411</v>
+        <v>428</v>
       </c>
       <c r="C382" s="20" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B383" s="20" t="s">
         <v>203</v>
@@ -8965,10 +8989,10 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B384" s="20" t="s">
-        <v>203</v>
+        <v>431</v>
       </c>
       <c r="C384" s="20" t="s">
         <v>412</v>
@@ -8976,10 +9000,10 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B385" s="20" t="s">
-        <v>424</v>
+        <v>203</v>
       </c>
       <c r="C385" s="20" t="s">
         <v>412</v>
@@ -8987,54 +9011,54 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B386" s="20" t="s">
-        <v>438</v>
+        <v>411</v>
       </c>
       <c r="C386" s="20" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B387" s="20" t="s">
-        <v>440</v>
+        <v>203</v>
       </c>
       <c r="C387" s="20" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="B388" s="20" t="s">
-        <v>442</v>
+        <v>203</v>
       </c>
       <c r="C388" s="20" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B389" s="20" t="s">
-        <v>444</v>
+        <v>424</v>
       </c>
       <c r="C389" s="20" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="B390" s="20" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="C390" s="20" t="s">
         <v>403</v>
@@ -9042,12 +9066,56 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
+        <v>439</v>
+      </c>
+      <c r="B391" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="C391" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>441</v>
+      </c>
+      <c r="B392" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="C392" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>443</v>
+      </c>
+      <c r="B393" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="C393" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>445</v>
+      </c>
+      <c r="B394" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="C394" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
         <v>447</v>
       </c>
-      <c r="B391" s="20" t="s">
+      <c r="B395" s="20" t="s">
         <v>448</v>
       </c>
-      <c r="C391" s="20" t="s">
+      <c r="C395" s="20" t="s">
         <v>403</v>
       </c>
     </row>
@@ -9213,55 +9281,55 @@
     <hyperlink ref="F183" r:id="rId158"/>
     <hyperlink ref="F184" r:id="rId159"/>
     <hyperlink ref="F185" r:id="rId160"/>
-    <hyperlink ref="F306" r:id="rId161"/>
-    <hyperlink ref="F311" r:id="rId162"/>
-    <hyperlink ref="F308" r:id="rId163"/>
-    <hyperlink ref="F312" r:id="rId164"/>
-    <hyperlink ref="F313" r:id="rId165"/>
-    <hyperlink ref="F314" r:id="rId166"/>
-    <hyperlink ref="F315" r:id="rId167"/>
-    <hyperlink ref="F324" r:id="rId168"/>
-    <hyperlink ref="F326" r:id="rId169"/>
-    <hyperlink ref="F327" r:id="rId170"/>
-    <hyperlink ref="F329" r:id="rId171"/>
-    <hyperlink ref="F342" r:id="rId172"/>
-    <hyperlink ref="F343" r:id="rId173"/>
-    <hyperlink ref="F347" r:id="rId174"/>
-    <hyperlink ref="F348" r:id="rId175"/>
-    <hyperlink ref="F352" r:id="rId176"/>
-    <hyperlink ref="F353" r:id="rId177"/>
-    <hyperlink ref="F357" r:id="rId178"/>
-    <hyperlink ref="F358" r:id="rId179"/>
-    <hyperlink ref="F309" r:id="rId180"/>
-    <hyperlink ref="F310" r:id="rId181"/>
-    <hyperlink ref="F316" r:id="rId182"/>
-    <hyperlink ref="F317" r:id="rId183"/>
-    <hyperlink ref="F318" r:id="rId184"/>
-    <hyperlink ref="F319" r:id="rId185"/>
-    <hyperlink ref="F320" r:id="rId186"/>
-    <hyperlink ref="F321" r:id="rId187"/>
-    <hyperlink ref="F322" r:id="rId188"/>
-    <hyperlink ref="F344" r:id="rId189"/>
-    <hyperlink ref="F349" r:id="rId190"/>
-    <hyperlink ref="F354" r:id="rId191"/>
-    <hyperlink ref="F359" r:id="rId192"/>
-    <hyperlink ref="F323" r:id="rId193"/>
-    <hyperlink ref="F325" r:id="rId194"/>
-    <hyperlink ref="F328" r:id="rId195"/>
-    <hyperlink ref="F307" r:id="rId196"/>
-    <hyperlink ref="F330" r:id="rId197"/>
-    <hyperlink ref="F331" r:id="rId198" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F332" r:id="rId199" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F333" r:id="rId200" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F334" r:id="rId201" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F335" r:id="rId202" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F336" r:id="rId203" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F337" r:id="rId204" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F338" r:id="rId205" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F339" r:id="rId206" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F340" r:id="rId207" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F341" r:id="rId208" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F362" r:id="rId209"/>
+    <hyperlink ref="F310" r:id="rId161"/>
+    <hyperlink ref="F315" r:id="rId162"/>
+    <hyperlink ref="F312" r:id="rId163"/>
+    <hyperlink ref="F316" r:id="rId164"/>
+    <hyperlink ref="F317" r:id="rId165"/>
+    <hyperlink ref="F318" r:id="rId166"/>
+    <hyperlink ref="F319" r:id="rId167"/>
+    <hyperlink ref="F328" r:id="rId168"/>
+    <hyperlink ref="F330" r:id="rId169"/>
+    <hyperlink ref="F331" r:id="rId170"/>
+    <hyperlink ref="F333" r:id="rId171"/>
+    <hyperlink ref="F346" r:id="rId172"/>
+    <hyperlink ref="F347" r:id="rId173"/>
+    <hyperlink ref="F351" r:id="rId174"/>
+    <hyperlink ref="F352" r:id="rId175"/>
+    <hyperlink ref="F356" r:id="rId176"/>
+    <hyperlink ref="F357" r:id="rId177"/>
+    <hyperlink ref="F361" r:id="rId178"/>
+    <hyperlink ref="F362" r:id="rId179"/>
+    <hyperlink ref="F313" r:id="rId180"/>
+    <hyperlink ref="F314" r:id="rId181"/>
+    <hyperlink ref="F320" r:id="rId182"/>
+    <hyperlink ref="F321" r:id="rId183"/>
+    <hyperlink ref="F322" r:id="rId184"/>
+    <hyperlink ref="F323" r:id="rId185"/>
+    <hyperlink ref="F324" r:id="rId186"/>
+    <hyperlink ref="F325" r:id="rId187"/>
+    <hyperlink ref="F326" r:id="rId188"/>
+    <hyperlink ref="F348" r:id="rId189"/>
+    <hyperlink ref="F353" r:id="rId190"/>
+    <hyperlink ref="F358" r:id="rId191"/>
+    <hyperlink ref="F363" r:id="rId192"/>
+    <hyperlink ref="F327" r:id="rId193"/>
+    <hyperlink ref="F329" r:id="rId194"/>
+    <hyperlink ref="F332" r:id="rId195"/>
+    <hyperlink ref="F311" r:id="rId196"/>
+    <hyperlink ref="F334" r:id="rId197"/>
+    <hyperlink ref="F335" r:id="rId198" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F336" r:id="rId199" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F337" r:id="rId200" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F338" r:id="rId201" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F339" r:id="rId202" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F340" r:id="rId203" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F341" r:id="rId204" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F342" r:id="rId205" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F343" r:id="rId206" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F344" r:id="rId207" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F345" r:id="rId208" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F366" r:id="rId209"/>
     <hyperlink ref="F178" r:id="rId210"/>
     <hyperlink ref="F189" r:id="rId211"/>
     <hyperlink ref="F154" r:id="rId212" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
@@ -9272,7 +9340,7 @@
     <hyperlink ref="F159" r:id="rId217" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
     <hyperlink ref="F160" r:id="rId218" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
     <hyperlink ref="F161" r:id="rId219" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
-    <hyperlink ref="F363" r:id="rId220"/>
+    <hyperlink ref="F367" r:id="rId220"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId221"/>

</xml_diff>

<commit_message>
Added pins for RST_N and BR_CLK. This will fully support an ethernet card pinout now.
</commit_message>
<xml_diff>
--- a/Manufacturing/V2/XMP16-V2-BOM.xlsx
+++ b/Manufacturing/V2/XMP16-V2-BOM.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="XMP16_03" localSheetId="0">Sheet1!$A$9:$C$395</definedName>
+    <definedName name="XMP16_03" localSheetId="0">Sheet1!$A$9:$C$397</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1963" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="629">
   <si>
     <t>ref</t>
   </si>
@@ -1908,6 +1908,18 @@
   </si>
   <si>
     <t>B_CLK_EN</t>
+  </si>
+  <si>
+    <t>P27</t>
+  </si>
+  <si>
+    <t>P28</t>
+  </si>
+  <si>
+    <t>BL_CLK</t>
+  </si>
+  <si>
+    <t>PIN_ARRAY_1x1</t>
   </si>
 </sst>
 </file>
@@ -2421,10 +2433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F395"/>
+  <dimension ref="A1:F397"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C199" sqref="C199"/>
+      <selection activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6119,38 +6131,32 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>206</v>
-      </c>
-      <c r="B200" t="s">
-        <v>207</v>
-      </c>
-      <c r="C200" t="s">
-        <v>212</v>
-      </c>
-      <c r="E200" s="24" t="s">
-        <v>541</v>
+        <v>625</v>
+      </c>
+      <c r="B200" s="20" t="s">
+        <v>627</v>
+      </c>
+      <c r="C200" s="20" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>208</v>
-      </c>
-      <c r="B201" t="s">
-        <v>209</v>
-      </c>
-      <c r="C201" t="s">
-        <v>212</v>
-      </c>
-      <c r="E201" s="24" t="s">
-        <v>541</v>
+        <v>626</v>
+      </c>
+      <c r="B201" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="C201" s="20" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B202" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C202" t="s">
         <v>212</v>
@@ -6161,10 +6167,10 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B203" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C203" t="s">
         <v>212</v>
@@ -6175,10 +6181,10 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B204" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C204" t="s">
         <v>212</v>
@@ -6189,10 +6195,10 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B205" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C205" t="s">
         <v>212</v>
@@ -6203,10 +6209,10 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B206" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C206" t="s">
         <v>212</v>
@@ -6217,10 +6223,10 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B207" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C207" t="s">
         <v>212</v>
@@ -6231,10 +6237,10 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B208" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="C208" t="s">
         <v>212</v>
@@ -6245,10 +6251,10 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B209" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C209" t="s">
         <v>212</v>
@@ -6259,7 +6265,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B210" t="s">
         <v>211</v>
@@ -6273,7 +6279,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B211" t="s">
         <v>211</v>
@@ -6287,7 +6293,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B212" t="s">
         <v>211</v>
@@ -6301,7 +6307,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B213" t="s">
         <v>211</v>
@@ -6315,7 +6321,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B214" t="s">
         <v>211</v>
@@ -6329,7 +6335,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B215" t="s">
         <v>211</v>
@@ -6343,10 +6349,10 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B216" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C216" t="s">
         <v>212</v>
@@ -6357,10 +6363,10 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B217" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="C217" t="s">
         <v>212</v>
@@ -6371,10 +6377,10 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B218" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C218" t="s">
         <v>212</v>
@@ -6385,10 +6391,10 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B219" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="C219" t="s">
         <v>212</v>
@@ -6399,10 +6405,10 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B220" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C220" t="s">
         <v>212</v>
@@ -6413,7 +6419,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B221" t="s">
         <v>221</v>
@@ -6427,7 +6433,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B222" t="s">
         <v>221</v>
@@ -6441,7 +6447,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B223" t="s">
         <v>221</v>
@@ -6455,10 +6461,10 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B224" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C224" t="s">
         <v>212</v>
@@ -6469,10 +6475,10 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B225" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C225" t="s">
         <v>212</v>
@@ -6483,10 +6489,10 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B226" t="s">
-        <v>242</v>
+        <v>211</v>
       </c>
       <c r="C226" t="s">
         <v>212</v>
@@ -6497,10 +6503,10 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B227" t="s">
-        <v>242</v>
+        <v>211</v>
       </c>
       <c r="C227" t="s">
         <v>212</v>
@@ -6511,10 +6517,10 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B228" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="C228" t="s">
         <v>212</v>
@@ -6525,10 +6531,10 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B229" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="C229" t="s">
         <v>212</v>
@@ -6539,7 +6545,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B230" t="s">
         <v>211</v>
@@ -6553,7 +6559,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B231" t="s">
         <v>211</v>
@@ -6567,7 +6573,7 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B232" t="s">
         <v>211</v>
@@ -6581,7 +6587,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B233" t="s">
         <v>211</v>
@@ -6595,7 +6601,7 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B234" t="s">
         <v>211</v>
@@ -6609,7 +6615,7 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B235" t="s">
         <v>211</v>
@@ -6623,7 +6629,7 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B236" t="s">
         <v>211</v>
@@ -6637,7 +6643,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B237" t="s">
         <v>211</v>
@@ -6651,7 +6657,7 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B238" t="s">
         <v>211</v>
@@ -6665,7 +6671,7 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B239" t="s">
         <v>211</v>
@@ -6679,7 +6685,7 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B240" t="s">
         <v>211</v>
@@ -6693,10 +6699,10 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B241" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="C241" t="s">
         <v>212</v>
@@ -6707,10 +6713,10 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B242" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C242" t="s">
         <v>212</v>
@@ -6721,10 +6727,10 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B243" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C243" t="s">
         <v>212</v>
@@ -6735,10 +6741,10 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B244" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="C244" t="s">
         <v>212</v>
@@ -6749,7 +6755,7 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B245" t="s">
         <v>261</v>
@@ -6763,7 +6769,7 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B246" t="s">
         <v>261</v>
@@ -6777,10 +6783,10 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B247" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C247" t="s">
         <v>212</v>
@@ -6791,7 +6797,7 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B248" t="s">
         <v>261</v>
@@ -6805,10 +6811,10 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B249" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C249" t="s">
         <v>212</v>
@@ -6819,7 +6825,7 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B250" t="s">
         <v>261</v>
@@ -6833,7 +6839,7 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B251" t="s">
         <v>261</v>
@@ -6847,10 +6853,10 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B252" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C252" t="s">
         <v>212</v>
@@ -6861,10 +6867,10 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B253" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C253" t="s">
         <v>212</v>
@@ -6875,10 +6881,10 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B254" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C254" t="s">
         <v>212</v>
@@ -6889,10 +6895,10 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B255" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C255" t="s">
         <v>212</v>
@@ -6903,10 +6909,10 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B256" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C256" t="s">
         <v>212</v>
@@ -6917,10 +6923,10 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B257" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="C257" t="s">
         <v>212</v>
@@ -6931,7 +6937,7 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B258" t="s">
         <v>261</v>
@@ -6945,7 +6951,7 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B259" t="s">
         <v>261</v>
@@ -6959,10 +6965,10 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B260" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C260" t="s">
         <v>212</v>
@@ -6973,7 +6979,7 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B261" t="s">
         <v>261</v>
@@ -6987,10 +6993,10 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B262" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C262" t="s">
         <v>212</v>
@@ -7001,7 +7007,7 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B263" t="s">
         <v>261</v>
@@ -7015,7 +7021,7 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B264" t="s">
         <v>261</v>
@@ -7029,10 +7035,10 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B265" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C265" t="s">
         <v>212</v>
@@ -7043,10 +7049,10 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B266" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C266" t="s">
         <v>212</v>
@@ -7057,10 +7063,10 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B267" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C267" t="s">
         <v>212</v>
@@ -7071,10 +7077,10 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B268" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C268" t="s">
         <v>212</v>
@@ -7085,10 +7091,10 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B269" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C269" t="s">
         <v>212</v>
@@ -7099,10 +7105,10 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B270" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="C270" t="s">
         <v>212</v>
@@ -7113,7 +7119,7 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B271" t="s">
         <v>261</v>
@@ -7127,7 +7133,7 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B272" t="s">
         <v>261</v>
@@ -7141,10 +7147,10 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B273" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C273" t="s">
         <v>212</v>
@@ -7155,7 +7161,7 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B274" t="s">
         <v>261</v>
@@ -7169,10 +7175,10 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B275" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C275" t="s">
         <v>212</v>
@@ -7183,7 +7189,7 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B276" t="s">
         <v>261</v>
@@ -7197,7 +7203,7 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B277" t="s">
         <v>261</v>
@@ -7211,10 +7217,10 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B278" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C278" t="s">
         <v>212</v>
@@ -7225,10 +7231,10 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B279" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C279" t="s">
         <v>212</v>
@@ -7239,10 +7245,10 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B280" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C280" t="s">
         <v>212</v>
@@ -7253,10 +7259,10 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B281" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C281" t="s">
         <v>212</v>
@@ -7267,10 +7273,10 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B282" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C282" t="s">
         <v>212</v>
@@ -7281,10 +7287,10 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B283" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="C283" t="s">
         <v>212</v>
@@ -7295,7 +7301,7 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B284" t="s">
         <v>261</v>
@@ -7309,7 +7315,7 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B285" t="s">
         <v>261</v>
@@ -7323,10 +7329,10 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B286" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C286" t="s">
         <v>212</v>
@@ -7337,7 +7343,7 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B287" t="s">
         <v>261</v>
@@ -7351,10 +7357,10 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B288" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C288" t="s">
         <v>212</v>
@@ -7365,7 +7371,7 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B289" t="s">
         <v>261</v>
@@ -7379,7 +7385,7 @@
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B290" t="s">
         <v>261</v>
@@ -7393,10 +7399,10 @@
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B291" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C291" t="s">
         <v>212</v>
@@ -7407,10 +7413,10 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B292" t="s">
-        <v>312</v>
+        <v>261</v>
       </c>
       <c r="C292" t="s">
         <v>212</v>
@@ -7421,10 +7427,10 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B293" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C293" t="s">
         <v>212</v>
@@ -7435,13 +7441,13 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B294" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C294" t="s">
-        <v>316</v>
+        <v>212</v>
       </c>
       <c r="E294" s="24" t="s">
         <v>541</v>
@@ -7449,13 +7455,13 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B295" t="s">
-        <v>315</v>
+        <v>261</v>
       </c>
       <c r="C295" t="s">
-        <v>316</v>
+        <v>212</v>
       </c>
       <c r="E295" s="24" t="s">
         <v>541</v>
@@ -7463,7 +7469,7 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B296" t="s">
         <v>315</v>
@@ -7477,7 +7483,7 @@
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B297" t="s">
         <v>315</v>
@@ -7491,7 +7497,7 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B298" t="s">
         <v>315</v>
@@ -7505,13 +7511,13 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B299" t="s">
-        <v>221</v>
+        <v>315</v>
       </c>
       <c r="C299" t="s">
-        <v>212</v>
+        <v>316</v>
       </c>
       <c r="E299" s="24" t="s">
         <v>541</v>
@@ -7519,35 +7525,35 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>606</v>
+        <v>320</v>
       </c>
       <c r="B300" t="s">
-        <v>261</v>
+        <v>315</v>
       </c>
       <c r="C300" t="s">
-        <v>212</v>
-      </c>
-      <c r="E300" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="E300" s="24" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>607</v>
+        <v>321</v>
       </c>
       <c r="B301" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="C301" t="s">
         <v>212</v>
       </c>
-      <c r="E301" s="41" t="s">
+      <c r="E301" s="24" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B302" t="s">
         <v>261</v>
@@ -7561,7 +7567,7 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B303" t="s">
         <v>261</v>
@@ -7575,7 +7581,7 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B304" t="s">
         <v>261</v>
@@ -7589,7 +7595,7 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B305" t="s">
         <v>261</v>
@@ -7603,7 +7609,7 @@
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B306" t="s">
         <v>261</v>
@@ -7617,7 +7623,7 @@
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B307" t="s">
         <v>261</v>
@@ -7631,10 +7637,10 @@
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B308" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C308" t="s">
         <v>212</v>
@@ -7645,175 +7651,163 @@
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
+        <v>613</v>
+      </c>
+      <c r="B309" t="s">
+        <v>261</v>
+      </c>
+      <c r="C309" t="s">
+        <v>212</v>
+      </c>
+      <c r="E309" s="41" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>614</v>
+      </c>
+      <c r="B310" t="s">
+        <v>211</v>
+      </c>
+      <c r="C310" t="s">
+        <v>212</v>
+      </c>
+      <c r="E310" s="41" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
         <v>615</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B311" t="s">
         <v>211</v>
       </c>
-      <c r="C309" t="s">
-        <v>212</v>
-      </c>
-      <c r="E309" s="41" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="310" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A310" t="s">
-        <v>322</v>
-      </c>
-      <c r="B310" t="s">
-        <v>542</v>
-      </c>
-      <c r="C310" t="s">
-        <v>324</v>
-      </c>
-      <c r="E310" s="25" t="s">
-        <v>543</v>
-      </c>
-      <c r="F310" s="26" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A311" t="s">
-        <v>325</v>
-      </c>
-      <c r="B311" t="s">
-        <v>326</v>
-      </c>
       <c r="C311" t="s">
-        <v>327</v>
-      </c>
-      <c r="D311" t="s">
-        <v>549</v>
-      </c>
-      <c r="E311" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F311" s="43" t="s">
-        <v>547</v>
+        <v>212</v>
+      </c>
+      <c r="E311" s="41" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="312" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B312" t="s">
-        <v>329</v>
+        <v>542</v>
       </c>
       <c r="C312" t="s">
-        <v>330</v>
-      </c>
-      <c r="E312" s="29" t="s">
-        <v>545</v>
-      </c>
-      <c r="F312" s="31" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="313" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="E312" s="25" t="s">
+        <v>543</v>
+      </c>
+      <c r="F312" s="26" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B313" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C313" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D313" t="s">
-        <v>552</v>
-      </c>
-      <c r="E313" s="32" t="s">
-        <v>550</v>
-      </c>
-      <c r="F313" s="33" t="s">
-        <v>551</v>
+        <v>549</v>
+      </c>
+      <c r="E313" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F313" s="43" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B314" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C314" t="s">
-        <v>336</v>
-      </c>
-      <c r="D314" t="s">
-        <v>555</v>
-      </c>
-      <c r="E314" s="34" t="s">
-        <v>553</v>
-      </c>
-      <c r="F314" s="35" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+      <c r="E314" s="29" t="s">
+        <v>545</v>
+      </c>
+      <c r="F314" s="31" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B315" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="C315" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="D315" t="s">
-        <v>556</v>
-      </c>
-      <c r="E315" s="27" t="s">
-        <v>543</v>
-      </c>
-      <c r="F315" s="28" t="s">
-        <v>544</v>
+        <v>552</v>
+      </c>
+      <c r="E315" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="F315" s="33" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="316" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B316" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="C316" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="D316" t="s">
-        <v>549</v>
-      </c>
-      <c r="E316" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F316" s="30" t="s">
-        <v>547</v>
+        <v>555</v>
+      </c>
+      <c r="E316" s="34" t="s">
+        <v>553</v>
+      </c>
+      <c r="F316" s="35" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="317" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B317" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C317" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D317" t="s">
-        <v>549</v>
-      </c>
-      <c r="E317" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F317" s="30" t="s">
-        <v>547</v>
+        <v>556</v>
+      </c>
+      <c r="E317" s="27" t="s">
+        <v>543</v>
+      </c>
+      <c r="F317" s="28" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="318" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B318" t="s">
         <v>326</v>
@@ -7833,7 +7827,7 @@
     </row>
     <row r="319" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B319" t="s">
         <v>326</v>
@@ -7853,67 +7847,67 @@
     </row>
     <row r="320" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B320" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="C320" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="D320" t="s">
-        <v>487</v>
-      </c>
-      <c r="E320" s="36" t="s">
-        <v>557</v>
-      </c>
-      <c r="F320" s="38" t="s">
-        <v>558</v>
+        <v>549</v>
+      </c>
+      <c r="E320" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F320" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="321" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B321" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="C321" t="s">
         <v>327</v>
       </c>
       <c r="D321" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="E321" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="F321" s="37" t="s">
-        <v>560</v>
+        <v>548</v>
+      </c>
+      <c r="F321" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="322" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B322" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C322" t="s">
-        <v>327</v>
+        <v>344</v>
       </c>
       <c r="D322" t="s">
-        <v>555</v>
-      </c>
-      <c r="E322" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="F322" s="37" t="s">
-        <v>560</v>
+        <v>487</v>
+      </c>
+      <c r="E322" s="36" t="s">
+        <v>557</v>
+      </c>
+      <c r="F322" s="38" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="323" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B323" t="s">
         <v>346</v>
@@ -7933,7 +7927,7 @@
     </row>
     <row r="324" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B324" t="s">
         <v>346</v>
@@ -7953,107 +7947,107 @@
     </row>
     <row r="325" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B325" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="C325" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D325" t="s">
         <v>555</v>
       </c>
-      <c r="E325" s="36" t="s">
-        <v>553</v>
-      </c>
-      <c r="F325" s="38" t="s">
-        <v>554</v>
+      <c r="E325" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F325" s="37" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="326" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B326" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C326" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="D326" t="s">
-        <v>563</v>
-      </c>
-      <c r="E326" s="39" t="s">
-        <v>561</v>
-      </c>
-      <c r="F326" s="40" t="s">
-        <v>562</v>
+        <v>555</v>
+      </c>
+      <c r="E326" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F326" s="37" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="327" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B327" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="C327" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="D327" t="s">
-        <v>565</v>
-      </c>
-      <c r="E327" s="41" t="s">
-        <v>355</v>
-      </c>
-      <c r="F327" s="42" t="s">
-        <v>564</v>
+        <v>555</v>
+      </c>
+      <c r="E327" s="36" t="s">
+        <v>553</v>
+      </c>
+      <c r="F327" s="38" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="328" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B328" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="C328" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="D328" t="s">
-        <v>549</v>
-      </c>
-      <c r="E328" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F328" s="30" t="s">
-        <v>547</v>
+        <v>563</v>
+      </c>
+      <c r="E328" s="39" t="s">
+        <v>561</v>
+      </c>
+      <c r="F328" s="40" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="329" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B329" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C329" t="s">
-        <v>327</v>
+        <v>356</v>
       </c>
       <c r="D329" t="s">
-        <v>549</v>
-      </c>
-      <c r="E329" s="44" t="s">
-        <v>566</v>
-      </c>
-      <c r="F329" s="45" t="s">
-        <v>567</v>
+        <v>565</v>
+      </c>
+      <c r="E329" s="41" t="s">
+        <v>355</v>
+      </c>
+      <c r="F329" s="42" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="330" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B330" t="s">
         <v>326</v>
@@ -8073,10 +8067,10 @@
     </row>
     <row r="331" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B331" t="s">
-        <v>326</v>
+        <v>359</v>
       </c>
       <c r="C331" t="s">
         <v>327</v>
@@ -8084,19 +8078,19 @@
       <c r="D331" t="s">
         <v>549</v>
       </c>
-      <c r="E331" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F331" s="30" t="s">
-        <v>547</v>
+      <c r="E331" s="44" t="s">
+        <v>566</v>
+      </c>
+      <c r="F331" s="45" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="332" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B332" t="s">
-        <v>359</v>
+        <v>326</v>
       </c>
       <c r="C332" t="s">
         <v>327</v>
@@ -8104,16 +8098,16 @@
       <c r="D332" t="s">
         <v>549</v>
       </c>
-      <c r="E332" s="44" t="s">
-        <v>566</v>
-      </c>
-      <c r="F332" s="45" t="s">
-        <v>567</v>
+      <c r="E332" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F332" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="333" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B333" t="s">
         <v>326</v>
@@ -8131,49 +8125,49 @@
         <v>547</v>
       </c>
     </row>
-    <row r="334" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B334" t="s">
-        <v>571</v>
+        <v>359</v>
       </c>
       <c r="C334" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
       <c r="D334" t="s">
-        <v>568</v>
-      </c>
-      <c r="E334" s="47" t="s">
-        <v>569</v>
-      </c>
-      <c r="F334" s="46" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="335" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+      <c r="E334" s="44" t="s">
+        <v>566</v>
+      </c>
+      <c r="F334" s="45" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B335" t="s">
-        <v>571</v>
+        <v>326</v>
       </c>
       <c r="C335" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
       <c r="D335" t="s">
-        <v>568</v>
-      </c>
-      <c r="E335" s="47" t="s">
-        <v>569</v>
-      </c>
-      <c r="F335" s="46" t="s">
-        <v>572</v>
+        <v>549</v>
+      </c>
+      <c r="E335" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F335" s="30" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="336" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B336" t="s">
         <v>571</v>
@@ -8188,12 +8182,12 @@
         <v>569</v>
       </c>
       <c r="F336" s="46" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="337" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B337" t="s">
         <v>571</v>
@@ -8208,12 +8202,12 @@
         <v>569</v>
       </c>
       <c r="F337" s="46" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="338" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B338" t="s">
         <v>571</v>
@@ -8228,12 +8222,12 @@
         <v>569</v>
       </c>
       <c r="F338" s="46" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="339" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B339" t="s">
         <v>571</v>
@@ -8248,12 +8242,12 @@
         <v>569</v>
       </c>
       <c r="F339" s="46" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="340" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B340" t="s">
         <v>571</v>
@@ -8268,12 +8262,12 @@
         <v>569</v>
       </c>
       <c r="F340" s="46" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="341" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B341" t="s">
         <v>571</v>
@@ -8288,12 +8282,12 @@
         <v>569</v>
       </c>
       <c r="F341" s="46" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="342" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B342" t="s">
         <v>571</v>
@@ -8308,12 +8302,12 @@
         <v>569</v>
       </c>
       <c r="F342" s="46" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="343" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B343" t="s">
         <v>571</v>
@@ -8328,12 +8322,12 @@
         <v>569</v>
       </c>
       <c r="F343" s="46" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="344" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B344" t="s">
         <v>571</v>
@@ -8348,12 +8342,12 @@
         <v>569</v>
       </c>
       <c r="F344" s="46" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="345" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B345" t="s">
         <v>571</v>
@@ -8368,551 +8362,569 @@
         <v>569</v>
       </c>
       <c r="F345" s="46" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>375</v>
+      </c>
+      <c r="B346" t="s">
+        <v>571</v>
+      </c>
+      <c r="C346" t="s">
+        <v>365</v>
+      </c>
+      <c r="D346" t="s">
+        <v>568</v>
+      </c>
+      <c r="E346" s="47" t="s">
+        <v>569</v>
+      </c>
+      <c r="F346" s="46" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>376</v>
+      </c>
+      <c r="B347" t="s">
+        <v>571</v>
+      </c>
+      <c r="C347" t="s">
+        <v>365</v>
+      </c>
+      <c r="D347" t="s">
+        <v>568</v>
+      </c>
+      <c r="E347" s="47" t="s">
+        <v>569</v>
+      </c>
+      <c r="F347" s="46" t="s">
         <v>582</v>
-      </c>
-    </row>
-    <row r="346" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A346" t="s">
-        <v>377</v>
-      </c>
-      <c r="B346" t="s">
-        <v>326</v>
-      </c>
-      <c r="C346" t="s">
-        <v>327</v>
-      </c>
-      <c r="D346" t="s">
-        <v>549</v>
-      </c>
-      <c r="E346" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F346" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="347" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A347" t="s">
-        <v>378</v>
-      </c>
-      <c r="B347" t="s">
-        <v>326</v>
-      </c>
-      <c r="C347" t="s">
-        <v>327</v>
-      </c>
-      <c r="D347" t="s">
-        <v>549</v>
-      </c>
-      <c r="E347" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F347" s="30" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="348" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
+        <v>377</v>
+      </c>
+      <c r="B348" t="s">
+        <v>326</v>
+      </c>
+      <c r="C348" t="s">
+        <v>327</v>
+      </c>
+      <c r="D348" t="s">
+        <v>549</v>
+      </c>
+      <c r="E348" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F348" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>378</v>
+      </c>
+      <c r="B349" t="s">
+        <v>326</v>
+      </c>
+      <c r="C349" t="s">
+        <v>327</v>
+      </c>
+      <c r="D349" t="s">
+        <v>549</v>
+      </c>
+      <c r="E349" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F349" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
         <v>379</v>
       </c>
-      <c r="B348" t="s">
+      <c r="B350" t="s">
         <v>352</v>
       </c>
-      <c r="C348" t="s">
+      <c r="C350" t="s">
         <v>353</v>
       </c>
-      <c r="D348" t="s">
+      <c r="D350" t="s">
         <v>563</v>
       </c>
-      <c r="E348" s="39" t="s">
+      <c r="E350" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F348" s="40" t="s">
+      <c r="F350" s="40" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A349" s="23" t="s">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="B349" s="23" t="s">
+      <c r="B351" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C349" s="23" t="s">
+      <c r="C351" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D349" s="23" t="s">
+      <c r="D351" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E349" s="23" t="s">
+      <c r="E351" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F349" s="23" t="s">
+      <c r="F351" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A350" s="23" t="s">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="B350" s="23" t="s">
+      <c r="B352" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C350" s="23" t="s">
+      <c r="C352" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D350" s="23" t="s">
+      <c r="D352" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E350" s="23" t="s">
+      <c r="E352" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F350" s="23" t="s">
+      <c r="F352" s="23" t="s">
         <v>584</v>
-      </c>
-    </row>
-    <row r="351" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A351" t="s">
-        <v>384</v>
-      </c>
-      <c r="B351" t="s">
-        <v>326</v>
-      </c>
-      <c r="C351" t="s">
-        <v>327</v>
-      </c>
-      <c r="D351" t="s">
-        <v>549</v>
-      </c>
-      <c r="E351" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F351" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="352" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A352" t="s">
-        <v>385</v>
-      </c>
-      <c r="B352" t="s">
-        <v>326</v>
-      </c>
-      <c r="C352" t="s">
-        <v>327</v>
-      </c>
-      <c r="D352" t="s">
-        <v>549</v>
-      </c>
-      <c r="E352" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F352" s="30" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="353" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
+        <v>384</v>
+      </c>
+      <c r="B353" t="s">
+        <v>326</v>
+      </c>
+      <c r="C353" t="s">
+        <v>327</v>
+      </c>
+      <c r="D353" t="s">
+        <v>549</v>
+      </c>
+      <c r="E353" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F353" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>385</v>
+      </c>
+      <c r="B354" t="s">
+        <v>326</v>
+      </c>
+      <c r="C354" t="s">
+        <v>327</v>
+      </c>
+      <c r="D354" t="s">
+        <v>549</v>
+      </c>
+      <c r="E354" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F354" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
         <v>386</v>
       </c>
-      <c r="B353" t="s">
+      <c r="B355" t="s">
         <v>352</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C355" t="s">
         <v>353</v>
       </c>
-      <c r="D353" t="s">
+      <c r="D355" t="s">
         <v>563</v>
       </c>
-      <c r="E353" s="39" t="s">
+      <c r="E355" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F353" s="40" t="s">
+      <c r="F355" s="40" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A354" s="23" t="s">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="B354" s="23" t="s">
+      <c r="B356" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C354" s="23" t="s">
+      <c r="C356" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D354" s="23" t="s">
+      <c r="D356" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E354" s="23" t="s">
+      <c r="E356" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F354" s="23" t="s">
+      <c r="F356" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A355" s="23" t="s">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="B355" s="23" t="s">
+      <c r="B357" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C355" s="23" t="s">
+      <c r="C357" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D355" s="23" t="s">
+      <c r="D357" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E355" s="23" t="s">
+      <c r="E357" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F355" s="23" t="s">
+      <c r="F357" s="23" t="s">
         <v>584</v>
-      </c>
-    </row>
-    <row r="356" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A356" t="s">
-        <v>389</v>
-      </c>
-      <c r="B356" t="s">
-        <v>326</v>
-      </c>
-      <c r="C356" t="s">
-        <v>327</v>
-      </c>
-      <c r="D356" t="s">
-        <v>549</v>
-      </c>
-      <c r="E356" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F356" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="357" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A357" t="s">
-        <v>390</v>
-      </c>
-      <c r="B357" t="s">
-        <v>326</v>
-      </c>
-      <c r="C357" t="s">
-        <v>327</v>
-      </c>
-      <c r="D357" t="s">
-        <v>549</v>
-      </c>
-      <c r="E357" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F357" s="30" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="358" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
+        <v>389</v>
+      </c>
+      <c r="B358" t="s">
+        <v>326</v>
+      </c>
+      <c r="C358" t="s">
+        <v>327</v>
+      </c>
+      <c r="D358" t="s">
+        <v>549</v>
+      </c>
+      <c r="E358" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F358" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>390</v>
+      </c>
+      <c r="B359" t="s">
+        <v>326</v>
+      </c>
+      <c r="C359" t="s">
+        <v>327</v>
+      </c>
+      <c r="D359" t="s">
+        <v>549</v>
+      </c>
+      <c r="E359" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F359" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
         <v>391</v>
       </c>
-      <c r="B358" t="s">
+      <c r="B360" t="s">
         <v>352</v>
       </c>
-      <c r="C358" t="s">
+      <c r="C360" t="s">
         <v>353</v>
       </c>
-      <c r="D358" t="s">
+      <c r="D360" t="s">
         <v>563</v>
       </c>
-      <c r="E358" s="39" t="s">
+      <c r="E360" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F358" s="40" t="s">
+      <c r="F360" s="40" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A359" s="23" t="s">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="B359" s="23" t="s">
+      <c r="B361" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C359" s="23" t="s">
+      <c r="C361" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D359" s="23" t="s">
+      <c r="D361" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E359" s="23" t="s">
+      <c r="E361" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F359" s="23" t="s">
+      <c r="F361" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A360" s="23" t="s">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="B360" s="23" t="s">
+      <c r="B362" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C360" s="23" t="s">
+      <c r="C362" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D360" s="23" t="s">
+      <c r="D362" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E360" s="23" t="s">
+      <c r="E362" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F360" s="23" t="s">
+      <c r="F362" s="23" t="s">
         <v>584</v>
-      </c>
-    </row>
-    <row r="361" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A361" t="s">
-        <v>394</v>
-      </c>
-      <c r="B361" t="s">
-        <v>326</v>
-      </c>
-      <c r="C361" t="s">
-        <v>327</v>
-      </c>
-      <c r="D361" t="s">
-        <v>549</v>
-      </c>
-      <c r="E361" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F361" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="362" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A362" t="s">
-        <v>395</v>
-      </c>
-      <c r="B362" t="s">
-        <v>326</v>
-      </c>
-      <c r="C362" t="s">
-        <v>327</v>
-      </c>
-      <c r="D362" t="s">
-        <v>549</v>
-      </c>
-      <c r="E362" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F362" s="30" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="363" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
+        <v>394</v>
+      </c>
+      <c r="B363" t="s">
+        <v>326</v>
+      </c>
+      <c r="C363" t="s">
+        <v>327</v>
+      </c>
+      <c r="D363" t="s">
+        <v>549</v>
+      </c>
+      <c r="E363" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F363" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>395</v>
+      </c>
+      <c r="B364" t="s">
+        <v>326</v>
+      </c>
+      <c r="C364" t="s">
+        <v>327</v>
+      </c>
+      <c r="D364" t="s">
+        <v>549</v>
+      </c>
+      <c r="E364" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F364" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
         <v>396</v>
       </c>
-      <c r="B363" t="s">
+      <c r="B365" t="s">
         <v>352</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C365" t="s">
         <v>353</v>
       </c>
-      <c r="D363" t="s">
+      <c r="D365" t="s">
         <v>563</v>
       </c>
-      <c r="E363" s="39" t="s">
+      <c r="E365" s="39" t="s">
         <v>561</v>
       </c>
-      <c r="F363" s="40" t="s">
+      <c r="F365" s="40" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A364" s="23" t="s">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="B364" s="23" t="s">
+      <c r="B366" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C364" s="23" t="s">
+      <c r="C366" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D364" s="23" t="s">
+      <c r="D366" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E364" s="23" t="s">
+      <c r="E366" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F364" s="23" t="s">
+      <c r="F366" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A365" s="23" t="s">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367" s="23" t="s">
         <v>398</v>
       </c>
-      <c r="B365" s="23" t="s">
+      <c r="B367" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="C365" s="23" t="s">
+      <c r="C367" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="D365" s="23" t="s">
+      <c r="D367" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="E365" s="23" t="s">
+      <c r="E367" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F365" s="23" t="s">
+      <c r="F367" s="23" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="366" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A366" t="s">
+    <row r="368" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
         <v>399</v>
       </c>
-      <c r="B366" t="s">
+      <c r="B368" t="s">
         <v>400</v>
       </c>
-      <c r="C366" t="s">
+      <c r="C368" t="s">
         <v>588</v>
       </c>
-      <c r="D366" t="s">
+      <c r="D368" t="s">
         <v>586</v>
       </c>
-      <c r="E366" s="49" t="s">
+      <c r="E368" s="49" t="s">
         <v>587</v>
       </c>
-      <c r="F366" s="48" t="s">
+      <c r="F368" s="48" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="367" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A367" t="s">
+    <row r="369" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
         <v>616</v>
       </c>
-      <c r="B367" t="s">
+      <c r="B369" t="s">
         <v>326</v>
       </c>
-      <c r="C367" t="s">
+      <c r="C369" t="s">
         <v>327</v>
       </c>
-      <c r="D367" t="s">
+      <c r="D369" t="s">
         <v>549</v>
       </c>
-      <c r="E367" s="3" t="s">
+      <c r="E369" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F367" s="48" t="s">
+      <c r="F369" s="48" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A368" t="s">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
         <v>401</v>
       </c>
-      <c r="B368" s="20" t="s">
+      <c r="B370" s="20" t="s">
         <v>402</v>
-      </c>
-      <c r="C368" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A369" t="s">
-        <v>404</v>
-      </c>
-      <c r="B369" s="20" t="s">
-        <v>405</v>
-      </c>
-      <c r="C369" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A370" t="s">
-        <v>406</v>
-      </c>
-      <c r="B370" s="20" t="s">
-        <v>407</v>
       </c>
       <c r="C370" s="20" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B371" s="20" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C371" s="20" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B372" s="20" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C372" s="20" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B373" s="20" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C373" s="20" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="B374" s="20" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C374" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
+        <v>413</v>
+      </c>
+      <c r="B375" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="C375" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>415</v>
+      </c>
+      <c r="B376" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="C376" s="20" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
         <v>417</v>
-      </c>
-      <c r="B375" s="20" t="s">
-        <v>418</v>
-      </c>
-      <c r="C375" s="20" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A376" t="s">
-        <v>419</v>
-      </c>
-      <c r="B376" s="20" t="s">
-        <v>420</v>
-      </c>
-      <c r="C376" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A377" t="s">
-        <v>421</v>
       </c>
       <c r="B377" s="20" t="s">
         <v>418</v>
@@ -8921,86 +8933,86 @@
         <v>412</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B378" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="C378" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>421</v>
+      </c>
+      <c r="B379" s="20" t="s">
         <v>418</v>
-      </c>
-      <c r="C378" s="20" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
-        <v>423</v>
-      </c>
-      <c r="B379" s="20" t="s">
-        <v>424</v>
       </c>
       <c r="C379" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B380" s="20" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C380" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B381" s="20" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C381" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B382" s="20" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C382" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B383" s="20" t="s">
-        <v>203</v>
+        <v>420</v>
       </c>
       <c r="C383" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B384" s="20" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C384" s="20" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B385" s="20" t="s">
         <v>203</v>
@@ -9011,10 +9023,10 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B386" s="20" t="s">
-        <v>411</v>
+        <v>431</v>
       </c>
       <c r="C386" s="20" t="s">
         <v>412</v>
@@ -9022,7 +9034,7 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B387" s="20" t="s">
         <v>203</v>
@@ -9033,10 +9045,10 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B388" s="20" t="s">
-        <v>203</v>
+        <v>411</v>
       </c>
       <c r="C388" s="20" t="s">
         <v>412</v>
@@ -9044,10 +9056,10 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B389" s="20" t="s">
-        <v>424</v>
+        <v>203</v>
       </c>
       <c r="C389" s="20" t="s">
         <v>412</v>
@@ -9055,32 +9067,32 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B390" s="20" t="s">
-        <v>438</v>
+        <v>203</v>
       </c>
       <c r="C390" s="20" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B391" s="20" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="C391" s="20" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B392" s="20" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C392" s="20" t="s">
         <v>403</v>
@@ -9088,10 +9100,10 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B393" s="20" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C393" s="20" t="s">
         <v>403</v>
@@ -9099,10 +9111,10 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B394" s="20" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C394" s="20" t="s">
         <v>403</v>
@@ -9110,12 +9122,34 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
+        <v>443</v>
+      </c>
+      <c r="B395" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="C395" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>445</v>
+      </c>
+      <c r="B396" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="C396" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
         <v>447</v>
       </c>
-      <c r="B395" s="20" t="s">
+      <c r="B397" s="20" t="s">
         <v>448</v>
       </c>
-      <c r="C395" s="20" t="s">
+      <c r="C397" s="20" t="s">
         <v>403</v>
       </c>
     </row>
@@ -9281,55 +9315,55 @@
     <hyperlink ref="F183" r:id="rId158"/>
     <hyperlink ref="F184" r:id="rId159"/>
     <hyperlink ref="F185" r:id="rId160"/>
-    <hyperlink ref="F310" r:id="rId161"/>
-    <hyperlink ref="F315" r:id="rId162"/>
-    <hyperlink ref="F312" r:id="rId163"/>
-    <hyperlink ref="F316" r:id="rId164"/>
-    <hyperlink ref="F317" r:id="rId165"/>
-    <hyperlink ref="F318" r:id="rId166"/>
-    <hyperlink ref="F319" r:id="rId167"/>
-    <hyperlink ref="F328" r:id="rId168"/>
-    <hyperlink ref="F330" r:id="rId169"/>
-    <hyperlink ref="F331" r:id="rId170"/>
-    <hyperlink ref="F333" r:id="rId171"/>
-    <hyperlink ref="F346" r:id="rId172"/>
-    <hyperlink ref="F347" r:id="rId173"/>
-    <hyperlink ref="F351" r:id="rId174"/>
-    <hyperlink ref="F352" r:id="rId175"/>
-    <hyperlink ref="F356" r:id="rId176"/>
-    <hyperlink ref="F357" r:id="rId177"/>
-    <hyperlink ref="F361" r:id="rId178"/>
-    <hyperlink ref="F362" r:id="rId179"/>
-    <hyperlink ref="F313" r:id="rId180"/>
-    <hyperlink ref="F314" r:id="rId181"/>
-    <hyperlink ref="F320" r:id="rId182"/>
-    <hyperlink ref="F321" r:id="rId183"/>
-    <hyperlink ref="F322" r:id="rId184"/>
-    <hyperlink ref="F323" r:id="rId185"/>
-    <hyperlink ref="F324" r:id="rId186"/>
-    <hyperlink ref="F325" r:id="rId187"/>
-    <hyperlink ref="F326" r:id="rId188"/>
-    <hyperlink ref="F348" r:id="rId189"/>
-    <hyperlink ref="F353" r:id="rId190"/>
-    <hyperlink ref="F358" r:id="rId191"/>
-    <hyperlink ref="F363" r:id="rId192"/>
-    <hyperlink ref="F327" r:id="rId193"/>
-    <hyperlink ref="F329" r:id="rId194"/>
-    <hyperlink ref="F332" r:id="rId195"/>
-    <hyperlink ref="F311" r:id="rId196"/>
-    <hyperlink ref="F334" r:id="rId197"/>
-    <hyperlink ref="F335" r:id="rId198" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F336" r:id="rId199" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F337" r:id="rId200" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F338" r:id="rId201" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F339" r:id="rId202" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F340" r:id="rId203" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F341" r:id="rId204" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F342" r:id="rId205" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F343" r:id="rId206" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F344" r:id="rId207" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F345" r:id="rId208" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
-    <hyperlink ref="F366" r:id="rId209"/>
+    <hyperlink ref="F312" r:id="rId161"/>
+    <hyperlink ref="F317" r:id="rId162"/>
+    <hyperlink ref="F314" r:id="rId163"/>
+    <hyperlink ref="F318" r:id="rId164"/>
+    <hyperlink ref="F319" r:id="rId165"/>
+    <hyperlink ref="F320" r:id="rId166"/>
+    <hyperlink ref="F321" r:id="rId167"/>
+    <hyperlink ref="F330" r:id="rId168"/>
+    <hyperlink ref="F332" r:id="rId169"/>
+    <hyperlink ref="F333" r:id="rId170"/>
+    <hyperlink ref="F335" r:id="rId171"/>
+    <hyperlink ref="F348" r:id="rId172"/>
+    <hyperlink ref="F349" r:id="rId173"/>
+    <hyperlink ref="F353" r:id="rId174"/>
+    <hyperlink ref="F354" r:id="rId175"/>
+    <hyperlink ref="F358" r:id="rId176"/>
+    <hyperlink ref="F359" r:id="rId177"/>
+    <hyperlink ref="F363" r:id="rId178"/>
+    <hyperlink ref="F364" r:id="rId179"/>
+    <hyperlink ref="F315" r:id="rId180"/>
+    <hyperlink ref="F316" r:id="rId181"/>
+    <hyperlink ref="F322" r:id="rId182"/>
+    <hyperlink ref="F323" r:id="rId183"/>
+    <hyperlink ref="F324" r:id="rId184"/>
+    <hyperlink ref="F325" r:id="rId185"/>
+    <hyperlink ref="F326" r:id="rId186"/>
+    <hyperlink ref="F327" r:id="rId187"/>
+    <hyperlink ref="F328" r:id="rId188"/>
+    <hyperlink ref="F350" r:id="rId189"/>
+    <hyperlink ref="F355" r:id="rId190"/>
+    <hyperlink ref="F360" r:id="rId191"/>
+    <hyperlink ref="F365" r:id="rId192"/>
+    <hyperlink ref="F329" r:id="rId193"/>
+    <hyperlink ref="F331" r:id="rId194"/>
+    <hyperlink ref="F334" r:id="rId195"/>
+    <hyperlink ref="F313" r:id="rId196"/>
+    <hyperlink ref="F336" r:id="rId197"/>
+    <hyperlink ref="F337" r:id="rId198" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F338" r:id="rId199" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F339" r:id="rId200" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F340" r:id="rId201" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F341" r:id="rId202" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F342" r:id="rId203" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F343" r:id="rId204" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F344" r:id="rId205" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F345" r:id="rId206" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F346" r:id="rId207" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F347" r:id="rId208" display="http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272"/>
+    <hyperlink ref="F368" r:id="rId209"/>
     <hyperlink ref="F178" r:id="rId210"/>
     <hyperlink ref="F189" r:id="rId211"/>
     <hyperlink ref="F154" r:id="rId212" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
@@ -9340,7 +9374,7 @@
     <hyperlink ref="F159" r:id="rId217" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
     <hyperlink ref="F160" r:id="rId218" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
     <hyperlink ref="F161" r:id="rId219" display="http://www.digikey.com/product-detail/en/LTST-C193KGKT-5A/160-1828-1-ND/2356247"/>
-    <hyperlink ref="F367" r:id="rId220"/>
+    <hyperlink ref="F369" r:id="rId220"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId221"/>

</xml_diff>

<commit_message>
Added second flash boot header --- attached to Mode4 pin on the flash-attached L2. The aim is to remove the need for any OTP work on this core, but it may be over-kill.
</commit_message>
<xml_diff>
--- a/Manufacturing/V2/XMP16-V2-BOM.xlsx
+++ b/Manufacturing/V2/XMP16-V2-BOM.xlsx
@@ -13,14 +13,14 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="XMP16_03" vbProcedure="false">Sheet1!$A$9:$C$399</definedName>
+    <definedName function="false" hidden="false" name="XMP16_03" vbProcedure="false">Sheet1!$A$9:$C$400</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1984" uniqueCount="636">
   <si>
     <t>XMP16-V2 BOM</t>
   </si>
@@ -1013,6 +1013,12 @@
   </si>
   <si>
     <t>BOOT_SPEED</t>
+  </si>
+  <si>
+    <t>P30</t>
+  </si>
+  <si>
+    <t>Flash_Boot2</t>
   </si>
   <si>
     <t>R1</t>
@@ -2283,10 +2289,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F399"/>
+  <dimension ref="A1:F400"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A189" view="normal" windowProtection="false" workbookViewId="0" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="100">
-      <selection activeCell="C203" activeCellId="0" pane="topLeft" sqref="C203"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A197" view="normal" windowProtection="false" workbookViewId="0" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="100">
+      <selection activeCell="B204" activeCellId="0" pane="topLeft" sqref="B204"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -6016,28 +6022,25 @@
       <c r="A203" s="0" t="s">
         <v>331</v>
       </c>
-      <c r="B203" s="0" t="s">
+      <c r="B203" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="C203" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E203" s="12" t="s">
-        <v>333</v>
+      <c r="C203" s="5" t="s">
+        <v>293</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="204">
       <c r="A204" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B204" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="B204" s="0" t="s">
-        <v>335</v>
-      </c>
       <c r="C204" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E204" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="205">
@@ -6051,7 +6054,7 @@
         <v>40</v>
       </c>
       <c r="E205" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="206">
@@ -6059,27 +6062,27 @@
         <v>338</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C206" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E206" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="207">
       <c r="A207" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B207" s="0" t="s">
         <v>339</v>
       </c>
-      <c r="B207" s="0" t="s">
-        <v>340</v>
-      </c>
       <c r="C207" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E207" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="208">
@@ -6093,7 +6096,7 @@
         <v>40</v>
       </c>
       <c r="E208" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="209">
@@ -6107,7 +6110,7 @@
         <v>40</v>
       </c>
       <c r="E209" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="210">
@@ -6121,7 +6124,7 @@
         <v>40</v>
       </c>
       <c r="E210" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="211">
@@ -6129,139 +6132,139 @@
         <v>347</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="C211" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E211" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="212">
       <c r="A212" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C212" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E212" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
       <c r="A213" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C213" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E213" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
       <c r="A214" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C214" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E214" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
       <c r="A215" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C215" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E215" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="216">
       <c r="A216" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C216" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E216" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="217">
       <c r="A217" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C217" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E217" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
       <c r="A218" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C218" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E218" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
       <c r="A219" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C219" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E219" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
       <c r="A220" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C220" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E220" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
@@ -6269,125 +6272,125 @@
         <v>358</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>342</v>
+        <v>359</v>
       </c>
       <c r="C221" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E221" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="222">
       <c r="A222" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C222" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E222" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
       <c r="A223" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C223" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E223" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
       <c r="A224" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C224" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E224" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
       <c r="A225" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C225" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E225" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="226">
       <c r="A226" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C226" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E226" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="227">
       <c r="A227" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="C227" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E227" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="228">
       <c r="A228" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E228" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="229">
       <c r="A229" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>367</v>
+        <v>339</v>
       </c>
       <c r="C229" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E229" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="230">
@@ -6395,209 +6398,209 @@
         <v>368</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E230" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="231">
       <c r="A231" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B231" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="B231" s="0" t="s">
-        <v>337</v>
-      </c>
       <c r="C231" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E231" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="232">
       <c r="A232" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E232" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="233">
       <c r="A233" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E233" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="234">
       <c r="A234" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E234" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="235">
       <c r="A235" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C235" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E235" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="236">
       <c r="A236" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C236" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E236" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="237">
       <c r="A237" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C237" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E237" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="238">
       <c r="A238" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B238" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C238" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E238" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="239">
       <c r="A239" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C239" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E239" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="240">
       <c r="A240" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C240" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E240" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="241">
       <c r="A241" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C241" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E241" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="242">
       <c r="A242" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C242" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E242" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="243">
       <c r="A243" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C243" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E243" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="244">
       <c r="A244" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>383</v>
+        <v>339</v>
       </c>
       <c r="C244" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E244" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="245">
@@ -6605,27 +6608,27 @@
         <v>384</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>342</v>
+        <v>385</v>
       </c>
       <c r="C245" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E245" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="246">
       <c r="A246" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>386</v>
+        <v>344</v>
       </c>
       <c r="C246" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E246" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="247">
@@ -6633,55 +6636,55 @@
         <v>387</v>
       </c>
       <c r="B247" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C247" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E247" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="248">
       <c r="A248" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B248" s="0" t="s">
         <v>388</v>
       </c>
-      <c r="B248" s="0" t="s">
-        <v>386</v>
-      </c>
       <c r="C248" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E248" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="249">
       <c r="A249" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B249" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C249" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E249" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="250">
       <c r="A250" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C250" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E250" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="251">
@@ -6689,629 +6692,629 @@
         <v>392</v>
       </c>
       <c r="B251" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="C251" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E251" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="252">
       <c r="A252" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C252" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E252" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="253">
       <c r="A253" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B253" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C253" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E253" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="254">
       <c r="A254" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B254" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C254" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E254" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="255">
       <c r="A255" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B255" s="0" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C255" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E255" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="256">
       <c r="A256" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B256" s="0" t="s">
-        <v>337</v>
+        <v>393</v>
       </c>
       <c r="C256" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E256" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="257">
       <c r="A257" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B257" s="0" t="s">
-        <v>383</v>
+        <v>339</v>
       </c>
       <c r="C257" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E257" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="258">
       <c r="A258" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B258" s="0" t="s">
-        <v>342</v>
+        <v>385</v>
       </c>
       <c r="C258" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E258" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="259">
       <c r="A259" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B259" s="0" t="s">
-        <v>386</v>
+        <v>344</v>
       </c>
       <c r="C259" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E259" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="260">
       <c r="A260" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B260" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C260" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E260" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="261">
       <c r="A261" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B261" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C261" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E261" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="262">
       <c r="A262" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B262" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C262" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E262" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="263">
       <c r="A263" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B263" s="0" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C263" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E263" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="264">
       <c r="A264" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B264" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="C264" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E264" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="265">
       <c r="A265" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B265" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C265" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E265" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="266">
       <c r="A266" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B266" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C266" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E266" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="267">
       <c r="A267" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B267" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C267" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E267" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="268">
       <c r="A268" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B268" s="0" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C268" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E268" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="269">
       <c r="A269" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B269" s="0" t="s">
-        <v>337</v>
+        <v>393</v>
       </c>
       <c r="C269" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E269" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="270">
       <c r="A270" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B270" s="0" t="s">
-        <v>383</v>
+        <v>339</v>
       </c>
       <c r="C270" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E270" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="271">
       <c r="A271" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B271" s="0" t="s">
-        <v>342</v>
+        <v>385</v>
       </c>
       <c r="C271" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E271" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="272">
       <c r="A272" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B272" s="0" t="s">
-        <v>386</v>
+        <v>344</v>
       </c>
       <c r="C272" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E272" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="273">
       <c r="A273" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B273" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C273" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E273" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="274">
       <c r="A274" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B274" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C274" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E274" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="275">
       <c r="A275" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B275" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C275" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E275" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="276">
       <c r="A276" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B276" s="0" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C276" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E276" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="277">
       <c r="A277" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B277" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="C277" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E277" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="278">
       <c r="A278" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B278" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C278" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E278" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="279">
       <c r="A279" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B279" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C279" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E279" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="280">
       <c r="A280" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B280" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C280" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E280" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="281">
       <c r="A281" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B281" s="0" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C281" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E281" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="282">
       <c r="A282" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B282" s="0" t="s">
-        <v>337</v>
+        <v>393</v>
       </c>
       <c r="C282" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E282" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="283">
       <c r="A283" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B283" s="0" t="s">
-        <v>383</v>
+        <v>339</v>
       </c>
       <c r="C283" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E283" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="284">
       <c r="A284" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B284" s="0" t="s">
-        <v>342</v>
+        <v>385</v>
       </c>
       <c r="C284" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E284" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="285">
       <c r="A285" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B285" s="0" t="s">
-        <v>386</v>
+        <v>344</v>
       </c>
       <c r="C285" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E285" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="286">
       <c r="A286" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B286" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C286" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E286" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="287">
       <c r="A287" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B287" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C287" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E287" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="288">
       <c r="A288" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B288" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C288" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E288" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="289">
       <c r="A289" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B289" s="0" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C289" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E289" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="290">
       <c r="A290" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B290" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="C290" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E290" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="291">
       <c r="A291" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B291" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C291" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E291" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="292">
       <c r="A292" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B292" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C292" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E292" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="293">
       <c r="A293" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B293" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C293" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E293" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="294">
       <c r="A294" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B294" s="0" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C294" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E294" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="295">
       <c r="A295" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B295" s="0" t="s">
-        <v>437</v>
+        <v>393</v>
       </c>
       <c r="C295" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E295" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="296">
@@ -7319,782 +7322,776 @@
         <v>438</v>
       </c>
       <c r="B296" s="0" t="s">
-        <v>386</v>
+        <v>439</v>
       </c>
       <c r="C296" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E296" s="12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="297">
+        <v>335</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="297">
       <c r="A297" s="0" t="s">
-        <v>439</v>
-      </c>
-      <c r="B297" s="15" t="s">
         <v>440</v>
       </c>
+      <c r="B297" s="0" t="s">
+        <v>388</v>
+      </c>
       <c r="C297" s="0" t="s">
-        <v>441</v>
-      </c>
-      <c r="D297" s="0" t="s">
-        <v>442</v>
-      </c>
-      <c r="E297" s="12"/>
-      <c r="F297" s="15" t="s">
-        <v>443</v>
+        <v>40</v>
+      </c>
+      <c r="E297" s="12" t="s">
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="298">
       <c r="A298" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="B298" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="C298" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="D298" s="0" t="s">
         <v>444</v>
-      </c>
-      <c r="B298" s="15" t="s">
-        <v>440</v>
-      </c>
-      <c r="C298" s="0" t="s">
-        <v>441</v>
-      </c>
-      <c r="D298" s="0" t="s">
-        <v>442</v>
       </c>
       <c r="E298" s="12"/>
       <c r="F298" s="15" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="299">
       <c r="A299" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B299" s="0" t="s">
-        <v>440</v>
+        <v>446</v>
+      </c>
+      <c r="B299" s="15" t="s">
+        <v>442</v>
       </c>
       <c r="C299" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D299" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E299" s="12"/>
       <c r="F299" s="15" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="300">
       <c r="A300" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B300" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C300" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D300" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E300" s="12"/>
       <c r="F300" s="15" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="301">
       <c r="A301" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B301" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C301" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D301" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E301" s="12"/>
       <c r="F301" s="15" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="302">
+      <c r="A302" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="B302" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C302" s="0" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="302">
-      <c r="A302" s="0" t="s">
-        <v>448</v>
-      </c>
-      <c r="B302" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="C302" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E302" s="12" t="s">
-        <v>333</v>
+      <c r="D302" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="E302" s="12"/>
+      <c r="F302" s="15" t="s">
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="303">
       <c r="A303" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B303" s="0" t="s">
-        <v>386</v>
+        <v>348</v>
       </c>
       <c r="C303" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E303" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="304">
       <c r="A304" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B304" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C304" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E304" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="305">
       <c r="A305" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B305" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C305" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E305" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="306">
       <c r="A306" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B306" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C306" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E306" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="307">
       <c r="A307" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B307" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C307" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E307" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="308">
       <c r="A308" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B308" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C308" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E308" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="309">
       <c r="A309" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B309" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C309" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E309" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="310">
       <c r="A310" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B310" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C310" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E310" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="311">
       <c r="A311" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B311" s="0" t="s">
-        <v>337</v>
+        <v>388</v>
       </c>
       <c r="C311" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E311" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="312">
       <c r="A312" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B312" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C312" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E312" s="12" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="313">
       <c r="A313" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B313" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C313" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E313" s="12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="314">
+        <v>335</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="314">
       <c r="A314" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B314" s="0" t="s">
-        <v>461</v>
+        <v>342</v>
       </c>
       <c r="C314" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="E314" s="11" t="s">
-        <v>463</v>
-      </c>
-      <c r="F314" s="9" t="s">
-        <v>464</v>
+        <v>40</v>
+      </c>
+      <c r="E314" s="12" t="s">
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="315">
       <c r="A315" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="B315" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="C315" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="E315" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="B315" s="0" t="s">
+      <c r="F315" s="9" t="s">
         <v>466</v>
-      </c>
-      <c r="C315" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D315" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E315" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="F315" s="9" t="s">
-        <v>470</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="316">
       <c r="A316" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="B316" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="C316" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D316" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E316" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="B316" s="0" t="s">
+      <c r="F316" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="C316" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="317">
+      <c r="A317" s="0" t="s">
         <v>473</v>
       </c>
-      <c r="E316" s="11" t="s">
+      <c r="B317" s="0" t="s">
         <v>474</v>
       </c>
-      <c r="F316" s="9" t="s">
+      <c r="C317" s="0" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="317">
-      <c r="A317" s="0" t="s">
+      <c r="E317" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="B317" s="0" t="s">
+      <c r="F317" s="9" t="s">
         <v>477</v>
       </c>
-      <c r="C317" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="318">
+      <c r="A318" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="D317" s="0" t="s">
+      <c r="B318" s="0" t="s">
         <v>479</v>
       </c>
-      <c r="E317" s="11" t="s">
+      <c r="C318" s="0" t="s">
         <v>480</v>
       </c>
-      <c r="F317" s="16" t="s">
+      <c r="D318" s="0" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="318">
-      <c r="A318" s="0" t="s">
+      <c r="E318" s="11" t="s">
         <v>482</v>
       </c>
-      <c r="B318" s="0" t="s">
+      <c r="F318" s="16" t="s">
         <v>483</v>
-      </c>
-      <c r="C318" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="D318" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="E318" s="11" t="s">
-        <v>486</v>
-      </c>
-      <c r="F318" s="9" t="s">
-        <v>487</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="319">
       <c r="A319" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="B319" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="C319" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="D319" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="E319" s="11" t="s">
         <v>488</v>
       </c>
-      <c r="B319" s="0" t="s">
+      <c r="F319" s="9" t="s">
         <v>489</v>
-      </c>
-      <c r="C319" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="D319" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="E319" s="11" t="s">
-        <v>463</v>
-      </c>
-      <c r="F319" s="9" t="s">
-        <v>464</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="320">
       <c r="A320" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="B320" s="0" t="s">
         <v>491</v>
       </c>
-      <c r="B320" s="0" t="s">
+      <c r="C320" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="D320" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="E320" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="F320" s="9" t="s">
         <v>466</v>
-      </c>
-      <c r="C320" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D320" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E320" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="F320" s="9" t="s">
-        <v>470</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="321">
       <c r="A321" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B321" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D321" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E321" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F321" s="9" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="322">
       <c r="A322" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B322" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D322" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E322" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F322" s="9" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="323">
       <c r="A323" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B323" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D323" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E323" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F323" s="9" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="324">
       <c r="A324" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B324" s="0" t="s">
-        <v>496</v>
+        <v>468</v>
       </c>
       <c r="C324" s="0" t="s">
-        <v>497</v>
+        <v>469</v>
       </c>
       <c r="D324" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="E324" s="11" t="s">
-        <v>498</v>
+        <v>470</v>
+      </c>
+      <c r="E324" s="8" t="s">
+        <v>471</v>
       </c>
       <c r="F324" s="9" t="s">
-        <v>499</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="325">
       <c r="A325" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="B325" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="C325" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="D325" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E325" s="11" t="s">
         <v>500</v>
       </c>
-      <c r="B325" s="0" t="s">
+      <c r="F325" s="9" t="s">
         <v>501</v>
-      </c>
-      <c r="C325" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D325" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="E325" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="F325" s="9" t="s">
-        <v>503</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="326">
       <c r="A326" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B326" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="C326" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D326" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="E326" s="8" t="s">
         <v>504</v>
       </c>
-      <c r="B326" s="0" t="s">
-        <v>501</v>
-      </c>
-      <c r="C326" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D326" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="E326" s="8" t="s">
-        <v>502</v>
-      </c>
       <c r="F326" s="9" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="327">
       <c r="A327" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="B327" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="C327" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D327" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="E327" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="F327" s="9" t="s">
         <v>505</v>
-      </c>
-      <c r="B327" s="0" t="s">
-        <v>501</v>
-      </c>
-      <c r="C327" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D327" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="E327" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="F327" s="9" t="s">
-        <v>503</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="328">
       <c r="A328" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B328" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C328" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D328" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E328" s="8" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="F328" s="9" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="329">
       <c r="A329" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B329" s="0" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="C329" s="0" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="D329" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="E329" s="11" t="s">
-        <v>486</v>
+        <v>487</v>
+      </c>
+      <c r="E329" s="8" t="s">
+        <v>504</v>
       </c>
       <c r="F329" s="9" t="s">
-        <v>487</v>
+        <v>505</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="330">
       <c r="A330" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B330" s="0" t="s">
-        <v>509</v>
+        <v>485</v>
       </c>
       <c r="C330" s="0" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="D330" s="0" t="s">
-        <v>511</v>
+        <v>487</v>
       </c>
       <c r="E330" s="11" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
       <c r="F330" s="9" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="331">
       <c r="A331" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="B331" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="C331" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="D331" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="E331" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="B331" s="0" t="s">
+      <c r="F331" s="9" t="s">
         <v>515</v>
-      </c>
-      <c r="C331" s="0" t="s">
-        <v>516</v>
-      </c>
-      <c r="D331" s="0" t="s">
-        <v>517</v>
-      </c>
-      <c r="E331" s="12" t="s">
-        <v>515</v>
-      </c>
-      <c r="F331" s="9" t="s">
-        <v>518</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="332">
       <c r="A332" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="B332" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="C332" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="D332" s="0" t="s">
         <v>519</v>
       </c>
-      <c r="B332" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="C332" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D332" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E332" s="8" t="s">
-        <v>469</v>
+      <c r="E332" s="12" t="s">
+        <v>517</v>
       </c>
       <c r="F332" s="9" t="s">
-        <v>470</v>
+        <v>520</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="333">
       <c r="A333" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B333" s="0" t="s">
-        <v>521</v>
+        <v>468</v>
       </c>
       <c r="C333" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D333" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E333" s="11" t="s">
-        <v>522</v>
+        <v>470</v>
+      </c>
+      <c r="E333" s="8" t="s">
+        <v>471</v>
       </c>
       <c r="F333" s="9" t="s">
-        <v>523</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="334">
       <c r="A334" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="B334" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="C334" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D334" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E334" s="11" t="s">
         <v>524</v>
       </c>
-      <c r="B334" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="C334" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D334" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E334" s="8" t="s">
-        <v>469</v>
-      </c>
       <c r="F334" s="9" t="s">
-        <v>470</v>
+        <v>525</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="335">
       <c r="A335" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B335" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D335" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E335" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F335" s="9" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="336">
       <c r="A336" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B336" s="0" t="s">
-        <v>521</v>
+        <v>468</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D336" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E336" s="11" t="s">
-        <v>522</v>
+        <v>470</v>
+      </c>
+      <c r="E336" s="8" t="s">
+        <v>471</v>
       </c>
       <c r="F336" s="9" t="s">
-        <v>523</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="337">
       <c r="A337" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B337" s="0" t="s">
-        <v>466</v>
+        <v>523</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D337" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E337" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="F337" s="9" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="338">
+      <c r="A338" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="B338" s="0" t="s">
         <v>468</v>
       </c>
-      <c r="E337" s="8" t="s">
+      <c r="C338" s="0" t="s">
         <v>469</v>
       </c>
-      <c r="F337" s="9" t="s">
+      <c r="D338" s="0" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="338">
-      <c r="A338" s="0" t="s">
-        <v>528</v>
-      </c>
-      <c r="B338" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="C338" s="0" t="s">
-        <v>530</v>
-      </c>
-      <c r="D338" s="0" t="s">
-        <v>531</v>
-      </c>
-      <c r="E338" s="17" t="s">
-        <v>532</v>
-      </c>
-      <c r="F338" s="16" t="s">
-        <v>533</v>
+      <c r="E338" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="F338" s="9" t="s">
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="339">
       <c r="A339" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="B339" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="C339" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="D339" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="E339" s="17" t="s">
         <v>534</v>
-      </c>
-      <c r="B339" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="C339" s="0" t="s">
-        <v>530</v>
-      </c>
-      <c r="D339" s="0" t="s">
-        <v>531</v>
-      </c>
-      <c r="E339" s="17" t="s">
-        <v>532</v>
       </c>
       <c r="F339" s="16" t="s">
         <v>535</v>
@@ -8105,16 +8102,16 @@
         <v>536</v>
       </c>
       <c r="B340" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D340" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E340" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F340" s="16" t="s">
         <v>537</v>
@@ -8125,16 +8122,16 @@
         <v>538</v>
       </c>
       <c r="B341" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D341" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E341" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F341" s="16" t="s">
         <v>539</v>
@@ -8145,16 +8142,16 @@
         <v>540</v>
       </c>
       <c r="B342" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C342" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D342" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E342" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F342" s="16" t="s">
         <v>541</v>
@@ -8165,16 +8162,16 @@
         <v>542</v>
       </c>
       <c r="B343" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D343" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E343" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F343" s="16" t="s">
         <v>543</v>
@@ -8185,16 +8182,16 @@
         <v>544</v>
       </c>
       <c r="B344" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C344" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D344" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E344" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F344" s="16" t="s">
         <v>545</v>
@@ -8205,16 +8202,16 @@
         <v>546</v>
       </c>
       <c r="B345" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D345" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E345" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F345" s="16" t="s">
         <v>547</v>
@@ -8225,16 +8222,16 @@
         <v>548</v>
       </c>
       <c r="B346" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D346" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E346" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F346" s="16" t="s">
         <v>549</v>
@@ -8245,16 +8242,16 @@
         <v>550</v>
       </c>
       <c r="B347" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C347" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D347" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E347" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F347" s="16" t="s">
         <v>551</v>
@@ -8265,16 +8262,16 @@
         <v>552</v>
       </c>
       <c r="B348" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C348" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D348" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E348" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F348" s="16" t="s">
         <v>553</v>
@@ -8285,481 +8282,490 @@
         <v>554</v>
       </c>
       <c r="B349" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D349" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E349" s="17" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F349" s="16" t="s">
         <v>555</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="350">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="350">
       <c r="A350" s="0" t="s">
         <v>556</v>
       </c>
       <c r="B350" s="0" t="s">
-        <v>466</v>
+        <v>531</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>467</v>
+        <v>532</v>
       </c>
       <c r="D350" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E350" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="F350" s="9" t="s">
-        <v>470</v>
+        <v>533</v>
+      </c>
+      <c r="E350" s="17" t="s">
+        <v>534</v>
+      </c>
+      <c r="F350" s="16" t="s">
+        <v>557</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="351">
       <c r="A351" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B351" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D351" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E351" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F351" s="9" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="352">
       <c r="A352" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B352" s="0" t="s">
-        <v>509</v>
+        <v>468</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>510</v>
+        <v>469</v>
       </c>
       <c r="D352" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E352" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="F352" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="353">
+      <c r="A353" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="B353" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="E352" s="11" t="s">
+      <c r="C353" s="0" t="s">
         <v>512</v>
       </c>
-      <c r="F352" s="9" t="s">
+      <c r="D353" s="0" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="353">
-      <c r="A353" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="B353" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="C353" s="6" t="s">
-        <v>561</v>
-      </c>
-      <c r="D353" s="6" t="s">
-        <v>562</v>
-      </c>
-      <c r="E353" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="F353" s="6" t="s">
-        <v>563</v>
+      <c r="E353" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="F353" s="9" t="s">
+        <v>515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="354">
       <c r="A354" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="B354" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C354" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="D354" s="6" t="s">
         <v>564</v>
       </c>
-      <c r="B354" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="C354" s="6" t="s">
-        <v>561</v>
-      </c>
-      <c r="D354" s="6" t="s">
+      <c r="E354" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="E354" s="6" t="s">
-        <v>560</v>
-      </c>
       <c r="F354" s="6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="355">
+      <c r="A355" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="B355" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C355" s="6" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="355">
-      <c r="A355" s="0" t="s">
+      <c r="D355" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="E355" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="F355" s="6" t="s">
         <v>565</v>
-      </c>
-      <c r="B355" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="C355" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D355" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E355" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="F355" s="9" t="s">
-        <v>470</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="356">
       <c r="A356" s="0" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B356" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C356" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D356" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E356" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F356" s="9" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="357">
       <c r="A357" s="0" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B357" s="0" t="s">
-        <v>509</v>
+        <v>468</v>
       </c>
       <c r="C357" s="0" t="s">
-        <v>510</v>
+        <v>469</v>
       </c>
       <c r="D357" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E357" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="F357" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="358">
+      <c r="A358" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="B358" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="E357" s="11" t="s">
+      <c r="C358" s="0" t="s">
         <v>512</v>
       </c>
-      <c r="F357" s="9" t="s">
+      <c r="D358" s="0" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="358">
-      <c r="A358" s="6" t="s">
-        <v>568</v>
-      </c>
-      <c r="B358" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="C358" s="6" t="s">
-        <v>561</v>
-      </c>
-      <c r="D358" s="6" t="s">
-        <v>562</v>
-      </c>
-      <c r="E358" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="F358" s="6" t="s">
-        <v>563</v>
+      <c r="E358" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="F358" s="9" t="s">
+        <v>515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="359">
       <c r="A359" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B359" s="6" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C359" s="6" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D359" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="E359" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="E359" s="6" t="s">
-        <v>560</v>
-      </c>
       <c r="F359" s="6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="360">
+      <c r="A360" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="B360" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C360" s="6" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="360">
-      <c r="A360" s="0" t="s">
-        <v>570</v>
-      </c>
-      <c r="B360" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="C360" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D360" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E360" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="F360" s="9" t="s">
-        <v>470</v>
+      <c r="D360" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="E360" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="F360" s="6" t="s">
+        <v>565</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="361">
       <c r="A361" s="0" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B361" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D361" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E361" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F361" s="9" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="362">
       <c r="A362" s="0" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B362" s="0" t="s">
-        <v>509</v>
+        <v>468</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>510</v>
+        <v>469</v>
       </c>
       <c r="D362" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E362" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="F362" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="363">
+      <c r="A363" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="B363" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="E362" s="11" t="s">
+      <c r="C363" s="0" t="s">
         <v>512</v>
       </c>
-      <c r="F362" s="9" t="s">
+      <c r="D363" s="0" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="363">
-      <c r="A363" s="6" t="s">
-        <v>573</v>
-      </c>
-      <c r="B363" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="C363" s="6" t="s">
-        <v>561</v>
-      </c>
-      <c r="D363" s="6" t="s">
-        <v>562</v>
-      </c>
-      <c r="E363" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="F363" s="6" t="s">
-        <v>563</v>
+      <c r="E363" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="F363" s="9" t="s">
+        <v>515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="364">
       <c r="A364" s="6" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B364" s="6" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C364" s="6" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D364" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="E364" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="E364" s="6" t="s">
-        <v>560</v>
-      </c>
       <c r="F364" s="6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="365">
+      <c r="A365" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B365" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C365" s="6" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="365">
-      <c r="A365" s="0" t="s">
-        <v>575</v>
-      </c>
-      <c r="B365" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="C365" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D365" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="E365" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="F365" s="9" t="s">
-        <v>470</v>
+      <c r="D365" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="E365" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="F365" s="6" t="s">
+        <v>565</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="366">
       <c r="A366" s="0" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B366" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C366" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D366" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E366" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F366" s="9" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="367">
       <c r="A367" s="0" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B367" s="0" t="s">
-        <v>509</v>
+        <v>468</v>
       </c>
       <c r="C367" s="0" t="s">
-        <v>510</v>
+        <v>469</v>
       </c>
       <c r="D367" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E367" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="F367" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="368">
+      <c r="A368" s="0" t="s">
+        <v>579</v>
+      </c>
+      <c r="B368" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="E367" s="11" t="s">
+      <c r="C368" s="0" t="s">
         <v>512</v>
       </c>
-      <c r="F367" s="9" t="s">
+      <c r="D368" s="0" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="368">
-      <c r="A368" s="6" t="s">
-        <v>578</v>
-      </c>
-      <c r="B368" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="C368" s="6" t="s">
-        <v>561</v>
-      </c>
-      <c r="D368" s="6" t="s">
-        <v>562</v>
-      </c>
-      <c r="E368" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="F368" s="6" t="s">
-        <v>563</v>
+      <c r="E368" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="F368" s="9" t="s">
+        <v>515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="369">
       <c r="A369" s="6" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B369" s="6" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C369" s="6" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D369" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="E369" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="E369" s="6" t="s">
-        <v>560</v>
-      </c>
       <c r="F369" s="6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="370">
+      <c r="A370" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="B370" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C370" s="6" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="370">
-      <c r="A370" s="0" t="s">
-        <v>580</v>
-      </c>
-      <c r="B370" s="0" t="s">
-        <v>581</v>
-      </c>
-      <c r="C370" s="0" t="s">
-        <v>582</v>
-      </c>
-      <c r="D370" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="E370" s="14" t="s">
-        <v>584</v>
-      </c>
-      <c r="F370" s="9" t="s">
-        <v>585</v>
+      <c r="D370" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="E370" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="F370" s="6" t="s">
+        <v>565</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="371">
       <c r="A371" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="B371" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="C371" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="D371" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="E371" s="14" t="s">
         <v>586</v>
       </c>
-      <c r="B371" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="C371" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D371" s="0" t="s">
+      <c r="F371" s="9" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="372">
+      <c r="A372" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="B372" s="0" t="s">
         <v>468</v>
       </c>
-      <c r="E371" s="8" t="s">
+      <c r="C372" s="0" t="s">
         <v>469</v>
       </c>
-      <c r="F371" s="9" t="s">
+      <c r="D372" s="0" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="372">
-      <c r="A372" s="0" t="s">
-        <v>587</v>
-      </c>
-      <c r="B372" s="5" t="s">
-        <v>588</v>
-      </c>
-      <c r="C372" s="5" t="s">
-        <v>589</v>
+      <c r="E372" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="F372" s="9" t="s">
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="373">
       <c r="A373" s="0" t="s">
+        <v>589</v>
+      </c>
+      <c r="B373" s="5" t="s">
         <v>590</v>
       </c>
-      <c r="B373" s="5" t="s">
+      <c r="C373" s="5" t="s">
         <v>591</v>
-      </c>
-      <c r="C373" s="5" t="s">
-        <v>589</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="374">
@@ -8770,7 +8776,7 @@
         <v>593</v>
       </c>
       <c r="C374" s="5" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="375">
@@ -8781,7 +8787,7 @@
         <v>595</v>
       </c>
       <c r="C375" s="5" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="376">
@@ -8792,18 +8798,18 @@
         <v>597</v>
       </c>
       <c r="C376" s="5" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="377">
       <c r="A377" s="0" t="s">
+        <v>598</v>
+      </c>
+      <c r="B377" s="5" t="s">
         <v>599</v>
       </c>
-      <c r="B377" s="5" t="s">
+      <c r="C377" s="5" t="s">
         <v>600</v>
-      </c>
-      <c r="C377" s="5" t="s">
-        <v>589</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="378">
@@ -8814,7 +8820,7 @@
         <v>602</v>
       </c>
       <c r="C378" s="5" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="379">
@@ -8825,7 +8831,7 @@
         <v>604</v>
       </c>
       <c r="C379" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="380">
@@ -8833,43 +8839,43 @@
         <v>605</v>
       </c>
       <c r="B380" s="5" t="s">
-        <v>328</v>
+        <v>606</v>
       </c>
       <c r="C380" s="5" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="381">
       <c r="A381" s="0" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B381" s="5" t="s">
-        <v>604</v>
+        <v>328</v>
       </c>
       <c r="C381" s="5" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="382">
       <c r="A382" s="0" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B382" s="5" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C382" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="383">
       <c r="A383" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B383" s="5" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C383" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="384">
@@ -8877,32 +8883,32 @@
         <v>610</v>
       </c>
       <c r="B384" s="5" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C384" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="385">
       <c r="A385" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="B385" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="B385" s="5" t="s">
-        <v>328</v>
-      </c>
       <c r="C385" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="386">
       <c r="A386" s="0" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B386" s="5" t="s">
-        <v>613</v>
+        <v>328</v>
       </c>
       <c r="C386" s="5" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="387">
@@ -8910,21 +8916,21 @@
         <v>614</v>
       </c>
       <c r="B387" s="5" t="s">
-        <v>313</v>
+        <v>615</v>
       </c>
       <c r="C387" s="5" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="388">
       <c r="A388" s="0" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>616</v>
+        <v>313</v>
       </c>
       <c r="C388" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="389">
@@ -8932,65 +8938,65 @@
         <v>617</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>313</v>
+        <v>618</v>
       </c>
       <c r="C389" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="390">
       <c r="A390" s="0" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B390" s="5" t="s">
-        <v>597</v>
+        <v>313</v>
       </c>
       <c r="C390" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="391">
       <c r="A391" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B391" s="5" t="s">
-        <v>313</v>
+        <v>599</v>
       </c>
       <c r="C391" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="392">
       <c r="A392" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B392" s="5" t="s">
         <v>313</v>
       </c>
       <c r="C392" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="393">
       <c r="A393" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B393" s="5" t="s">
-        <v>609</v>
+        <v>313</v>
       </c>
       <c r="C393" s="5" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="394">
       <c r="A394" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B394" s="5" t="s">
-        <v>623</v>
+        <v>611</v>
       </c>
       <c r="C394" s="5" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="395">
@@ -9001,7 +9007,7 @@
         <v>625</v>
       </c>
       <c r="C395" s="5" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="396">
@@ -9012,7 +9018,7 @@
         <v>627</v>
       </c>
       <c r="C396" s="5" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="397">
@@ -9023,7 +9029,7 @@
         <v>629</v>
       </c>
       <c r="C397" s="5" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="398">
@@ -9034,7 +9040,7 @@
         <v>631</v>
       </c>
       <c r="C398" s="5" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="399">
@@ -9045,7 +9051,18 @@
         <v>633</v>
       </c>
       <c r="C399" s="5" t="s">
-        <v>589</v>
+        <v>591</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="400">
+      <c r="A400" s="0" t="s">
+        <v>634</v>
+      </c>
+      <c r="B400" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="C400" s="5" t="s">
+        <v>591</v>
       </c>
     </row>
   </sheetData>
@@ -9220,61 +9237,61 @@
     <hyperlink display=" http://www.toby.co.uk/content/catalogue/products.aspx?series=FFC5-xx-R-L-Tx " ref="F184" r:id="rId168"/>
     <hyperlink display=" http://www.toby.co.uk/content/catalogue/products.aspx?series=FFC5-xx-R-L-Tx " ref="F185" r:id="rId169"/>
     <hyperlink display=" http://uk.farnell.com/harwin/m20-9990246/header-1row-2way/dp/1022247 " ref="F189" r:id="rId170"/>
-    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F297" r:id="rId171"/>
-    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F298" r:id="rId172"/>
-    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F299" r:id="rId173"/>
-    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F300" r:id="rId174"/>
-    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F301" r:id="rId175"/>
-    <hyperlink display=" http://search.digikey.com/uk/en/products/APX803-31SRG-7/APX803-31SRG-7DICT-ND/2285948 " ref="F314" r:id="rId176"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F315" r:id="rId177"/>
-    <hyperlink display=" http://search.digikey.com/uk/en/products/ASE-25.000MHZ-ET/535-9987-1-ND/2001610 " ref="F316" r:id="rId178"/>
-    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=LT3480EDD%23PBF-ND " ref="F317" r:id="rId179"/>
-    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=296-6487-1-ND " ref="F318" r:id="rId180"/>
-    <hyperlink display=" http://search.digikey.com/uk/en/products/APX803-31SRG-7/APX803-31SRG-7DICT-ND/2285948 " ref="F319" r:id="rId181"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F320" r:id="rId182"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F321" r:id="rId183"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F322" r:id="rId184"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F323" r:id="rId185"/>
-    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=74AHC1GU04W5-7DICT-ND " ref="F324" r:id="rId186"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/SN74LVC1G18DCKR/296-15569-2-ND/571179 " ref="F325" r:id="rId187"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/SN74LVC1G18DCKR/296-15569-2-ND/571179 " ref="F326" r:id="rId188"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/SN74LVC1G18DCKR/296-15569-2-ND/571179 " ref="F327" r:id="rId189"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/SN74LVC1G18DCKR/296-15569-2-ND/571179 " ref="F328" r:id="rId190"/>
-    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=296-6487-1-ND " ref="F329" r:id="rId191"/>
-    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F330" r:id="rId192"/>
-    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=SW1026CT-ND " ref="F331" r:id="rId193"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F332" r:id="rId194"/>
-    <hyperlink display=" http://search.digikey.com/us/en/products/NC7WZ07P6X/NC7WZ07P6XCT-ND/965702 " ref="F333" r:id="rId195"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F334" r:id="rId196"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F335" r:id="rId197"/>
-    <hyperlink display=" http://search.digikey.com/us/en/products/NC7WZ07P6X/NC7WZ07P6XCT-ND/965702 " ref="F336" r:id="rId198"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F337" r:id="rId199"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272 " ref="F338" r:id="rId200"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235273 " ref="F339" r:id="rId201"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235274 " ref="F340" r:id="rId202"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235275 " ref="F341" r:id="rId203"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235276 " ref="F342" r:id="rId204"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235277 " ref="F343" r:id="rId205"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235278 " ref="F344" r:id="rId206"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235279 " ref="F345" r:id="rId207"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235280 " ref="F346" r:id="rId208"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235281 " ref="F347" r:id="rId209"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235282 " ref="F348" r:id="rId210"/>
-    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235283 " ref="F349" r:id="rId211"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F350" r:id="rId212"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F351" r:id="rId213"/>
-    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F352" r:id="rId214"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F355" r:id="rId215"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F356" r:id="rId216"/>
-    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F357" r:id="rId217"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F360" r:id="rId218"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F361" r:id="rId219"/>
-    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F362" r:id="rId220"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F365" r:id="rId221"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F366" r:id="rId222"/>
-    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F367" r:id="rId223"/>
-    <hyperlink display=" http://uk.farnell.com/spansion/s25fl064k0smfi011/memory-flash-64m-3v-spi-8soic/dp/1861631?Ntt=S25FL064K " ref="F370" r:id="rId224"/>
-    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F371" r:id="rId225"/>
+    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F298" r:id="rId171"/>
+    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F299" r:id="rId172"/>
+    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F300" r:id="rId173"/>
+    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F301" r:id="rId174"/>
+    <hyperlink display="http://uk.farnell.com/bourns/crm0805-fx-r100elf/resistor-0805-0r1-1/dp/1865233RL" ref="F302" r:id="rId175"/>
+    <hyperlink display=" http://search.digikey.com/uk/en/products/APX803-31SRG-7/APX803-31SRG-7DICT-ND/2285948 " ref="F315" r:id="rId176"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F316" r:id="rId177"/>
+    <hyperlink display=" http://search.digikey.com/uk/en/products/ASE-25.000MHZ-ET/535-9987-1-ND/2001610 " ref="F317" r:id="rId178"/>
+    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=LT3480EDD%23PBF-ND " ref="F318" r:id="rId179"/>
+    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=296-6487-1-ND " ref="F319" r:id="rId180"/>
+    <hyperlink display=" http://search.digikey.com/uk/en/products/APX803-31SRG-7/APX803-31SRG-7DICT-ND/2285948 " ref="F320" r:id="rId181"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F321" r:id="rId182"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F322" r:id="rId183"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F323" r:id="rId184"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F324" r:id="rId185"/>
+    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=74AHC1GU04W5-7DICT-ND " ref="F325" r:id="rId186"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/SN74LVC1G18DCKR/296-15569-2-ND/571179 " ref="F326" r:id="rId187"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/SN74LVC1G18DCKR/296-15569-2-ND/571179 " ref="F327" r:id="rId188"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/SN74LVC1G18DCKR/296-15569-2-ND/571179 " ref="F328" r:id="rId189"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/SN74LVC1G18DCKR/296-15569-2-ND/571179 " ref="F329" r:id="rId190"/>
+    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=296-6487-1-ND " ref="F330" r:id="rId191"/>
+    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F331" r:id="rId192"/>
+    <hyperlink display=" http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=SW1026CT-ND " ref="F332" r:id="rId193"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F333" r:id="rId194"/>
+    <hyperlink display=" http://search.digikey.com/us/en/products/NC7WZ07P6X/NC7WZ07P6XCT-ND/965702 " ref="F334" r:id="rId195"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F335" r:id="rId196"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F336" r:id="rId197"/>
+    <hyperlink display=" http://search.digikey.com/us/en/products/NC7WZ07P6X/NC7WZ07P6XCT-ND/965702 " ref="F337" r:id="rId198"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F338" r:id="rId199"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235272 " ref="F339" r:id="rId200"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235273 " ref="F340" r:id="rId201"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235274 " ref="F341" r:id="rId202"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235275 " ref="F342" r:id="rId203"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235276 " ref="F343" r:id="rId204"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235277 " ref="F344" r:id="rId205"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235278 " ref="F345" r:id="rId206"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235279 " ref="F346" r:id="rId207"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235280 " ref="F347" r:id="rId208"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235281 " ref="F348" r:id="rId209"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235282 " ref="F349" r:id="rId210"/>
+    <hyperlink display=" http://uk.farnell.com/yageo-phycomp/yc124-jr-0733rl/resistor-array-arv341-0804-33r/dp/9235283 " ref="F350" r:id="rId211"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F351" r:id="rId212"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F352" r:id="rId213"/>
+    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F353" r:id="rId214"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F356" r:id="rId215"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F357" r:id="rId216"/>
+    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F358" r:id="rId217"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F361" r:id="rId218"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F362" r:id="rId219"/>
+    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F363" r:id="rId220"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F366" r:id="rId221"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F367" r:id="rId222"/>
+    <hyperlink display=" http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444 " ref="F368" r:id="rId223"/>
+    <hyperlink display=" http://uk.farnell.com/spansion/s25fl064k0smfi011/memory-flash-64m-3v-spi-8soic/dp/1861631?Ntt=S25FL064K " ref="F371" r:id="rId224"/>
+    <hyperlink display=" http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD " ref="F372" r:id="rId225"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>